<commit_message>
Forgot to add filtering to one of the tabs
Can now filter all of the stats for each tab at the bottom left.
</commit_message>
<xml_diff>
--- a/stats_workbook.xlsx
+++ b/stats_workbook.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\westw\Documents\8_2023_Spring\EENG311_Information Systems Science 2\ISSII_Group3Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4A994781-8876-4373-A5AE-1E48929F5392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D8A3DF6E-2044-4C13-BF86-200141201ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="21705"/>
   </bookViews>
   <sheets>
     <sheet name="stats" sheetId="1" r:id="rId1"/>
-    <sheet name="NAR" sheetId="4" r:id="rId2"/>
+    <sheet name="LSTM Multi" sheetId="2" r:id="rId2"/>
     <sheet name="NN_NoLSTM" sheetId="3" r:id="rId3"/>
-    <sheet name="LSTM Multi" sheetId="2" r:id="rId4"/>
+    <sheet name="NAR" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'LSTM Multi'!$A$1:$E$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NAR!$A$2:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'LSTM Multi'!$A$2:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">NAR!$A$2:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NN_NoLSTM!$A$2:$G$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stats!$A$26:$E$40</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="34">
   <si>
     <t>LSTM_Multichannel</t>
   </si>
@@ -613,7 +614,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -623,6 +624,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -982,7 +986,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,31 +1696,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1724,256 +1724,174 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.79727000000000003</v>
+        <v>0.81222000000000005</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>250</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0.73</v>
+        <v>0.70667000000000002</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>250</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>0.72777999999999998</v>
+        <v>0.61973999999999996</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>250</v>
+      </c>
+      <c r="E5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>0.72777999999999998</v>
+        <v>0.61602000000000001</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>250</v>
+      </c>
+      <c r="E6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>0.72333000000000003</v>
+        <v>0.61231000000000002</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>250</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>0.72111000000000003</v>
+        <v>0.52297000000000005</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>250</v>
+      </c>
+      <c r="E8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>0.69333</v>
+        <v>0.52175000000000005</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>250</v>
+      </c>
+      <c r="E9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>0.60111000000000003</v>
+        <v>0.1099</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>250</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>0.59777999999999998</v>
+        <v>3.4299999999999997E-2</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.45695000000000002</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>0.43382999999999999</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0.40998000000000001</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.1133</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>4.2900000000000001E-2</v>
-      </c>
-      <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="2">
-        <v>4.3055555555555562E-2</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="5" t="b">
-        <v>1</v>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>250</v>
+      </c>
+      <c r="E11">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E16"/>
+  <autoFilter ref="A2:E11">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E11">
+      <sortCondition descending="1" ref="A2:A11"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1983,10 +1901,19 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -1994,25 +1921,25 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2224,201 +2151,295 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:G11"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0.81222000000000005</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0.79727000000000003</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-      <c r="D2">
-        <v>250</v>
-      </c>
-      <c r="E2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>0.70667000000000002</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C4" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.72777999999999998</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>250</v>
-      </c>
-      <c r="E3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0.61973999999999996</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C5" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.72777999999999998</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.72333000000000003</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.72111000000000003</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.69333</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.60111000000000003</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.59777999999999998</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.45695000000000002</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.43382999999999999</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.40998000000000001</v>
+      </c>
+      <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-      <c r="D4">
-        <v>250</v>
-      </c>
-      <c r="E4">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.61602000000000001</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>50</v>
-      </c>
-      <c r="D5">
-        <v>250</v>
-      </c>
-      <c r="E5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.61231000000000002</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-      <c r="D6">
-        <v>250</v>
-      </c>
-      <c r="E6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.52297000000000005</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>100</v>
-      </c>
-      <c r="D7">
-        <v>250</v>
-      </c>
-      <c r="E7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.52175000000000005</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>50</v>
-      </c>
-      <c r="D8">
-        <v>250</v>
-      </c>
-      <c r="E8">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.1099</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C14" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.1133</v>
+      </c>
+      <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C9">
-        <v>100</v>
-      </c>
-      <c r="D9">
-        <v>250</v>
-      </c>
-      <c r="E9">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>3.4299999999999997E-2</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C15" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-      <c r="D10">
-        <v>250</v>
-      </c>
-      <c r="E10">
-        <v>150</v>
+      <c r="C16" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E10">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E10">
-      <sortCondition descending="1" ref="A1:A10"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A2:E16"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added an all stats tab/page
Can now filter all of our results and quickly pull the best results.
</commit_message>
<xml_diff>
--- a/stats_workbook.xlsx
+++ b/stats_workbook.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\westw\Documents\8_2023_Spring\EENG311_Information Systems Science 2\ISSII_Group3Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D8A3DF6E-2044-4C13-BF86-200141201ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{26ABB9FD-BA8F-45F6-9433-81CC5514B5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="21705"/>
   </bookViews>
   <sheets>
     <sheet name="stats" sheetId="1" r:id="rId1"/>
-    <sheet name="LSTM Multi" sheetId="2" r:id="rId2"/>
-    <sheet name="NN_NoLSTM" sheetId="3" r:id="rId3"/>
-    <sheet name="NAR" sheetId="4" r:id="rId4"/>
+    <sheet name="All Stats" sheetId="5" r:id="rId2"/>
+    <sheet name="LSTM Multi" sheetId="2" r:id="rId3"/>
+    <sheet name="NN_NoLSTM" sheetId="3" r:id="rId4"/>
+    <sheet name="NAR" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'LSTM Multi'!$A$2:$E$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">NAR!$A$2:$E$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NN_NoLSTM!$A$2:$G$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'All Stats'!$A$2:$C$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'LSTM Multi'!$A$2:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">NAR!$A$2:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">NN_NoLSTM!$A$2:$G$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stats!$A$26:$E$40</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="37">
   <si>
     <t>LSTM_Multichannel</t>
   </si>
@@ -131,6 +133,15 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>All stats</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Best of</t>
   </si>
 </sst>
 </file>
@@ -983,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,9 +1008,13 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1008,7 +1023,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1024,8 +1039,18 @@
       <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.81222000000000005</v>
       </c>
@@ -1041,8 +1066,18 @@
       <c r="E3">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+      <c r="J3" s="1">
+        <v>0.81222000000000005</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.70667000000000002</v>
       </c>
@@ -1058,8 +1093,18 @@
       <c r="E4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1">
+        <v>0.70667000000000002</v>
+      </c>
+      <c r="K4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.61973999999999996</v>
       </c>
@@ -1075,8 +1120,18 @@
       <c r="E5">
         <v>150</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1">
+        <v>0.61973999999999996</v>
+      </c>
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.61602000000000001</v>
       </c>
@@ -1092,8 +1147,18 @@
       <c r="E6">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1">
+        <v>0.61602000000000001</v>
+      </c>
+      <c r="K6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.61231000000000002</v>
       </c>
@@ -1109,8 +1174,18 @@
       <c r="E7">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1">
+        <v>0.61231000000000002</v>
+      </c>
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.52297000000000005</v>
       </c>
@@ -1126,8 +1201,18 @@
       <c r="E8">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1">
+        <v>0.52297000000000005</v>
+      </c>
+      <c r="K8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.52175000000000005</v>
       </c>
@@ -1143,8 +1228,18 @@
       <c r="E9">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1">
+        <v>0.52175000000000005</v>
+      </c>
+      <c r="K9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.1099</v>
       </c>
@@ -1160,8 +1255,18 @@
       <c r="E10">
         <v>150</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" s="1"/>
+      <c r="J10" s="1">
+        <v>0.1099</v>
+      </c>
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3.4299999999999997E-2</v>
       </c>
@@ -1177,8 +1282,18 @@
       <c r="E11">
         <v>150</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1187,7 +1302,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -1209,8 +1324,18 @@
       <c r="G14" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.81667000000000001</v>
       </c>
@@ -1232,8 +1357,18 @@
       <c r="G15" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" s="1"/>
+      <c r="J15" s="1">
+        <v>0.81667000000000001</v>
+      </c>
+      <c r="K15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.81444000000000005</v>
       </c>
@@ -1255,8 +1390,18 @@
       <c r="G16" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1">
+        <v>0.81444000000000005</v>
+      </c>
+      <c r="K16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0.81444000000000005</v>
       </c>
@@ -1278,8 +1423,18 @@
       <c r="G17" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1">
+        <v>0.81444000000000005</v>
+      </c>
+      <c r="K17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0.60133999999999999</v>
       </c>
@@ -1301,8 +1456,18 @@
       <c r="G18" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+      <c r="J18" s="1">
+        <v>0.60133999999999999</v>
+      </c>
+      <c r="K18" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0.51415</v>
       </c>
@@ -1324,8 +1489,18 @@
       <c r="G19" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="1"/>
+      <c r="J19" s="1">
+        <v>0.51415</v>
+      </c>
+      <c r="K19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0.50927999999999995</v>
       </c>
@@ -1347,8 +1522,18 @@
       <c r="G20" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+      <c r="J20" s="1">
+        <v>0.50927999999999995</v>
+      </c>
+      <c r="K20" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0.46516999999999997</v>
       </c>
@@ -1370,8 +1555,18 @@
       <c r="G21" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
+      <c r="J21" s="1">
+        <v>0.46516999999999997</v>
+      </c>
+      <c r="K21" t="s">
+        <v>25</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>0.1105</v>
       </c>
@@ -1393,8 +1588,18 @@
       <c r="G22" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1">
+        <v>0.1105</v>
+      </c>
+      <c r="K22" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2.5399999999999999E-2</v>
       </c>
@@ -1416,11 +1621,21 @@
       <c r="G23" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" s="1"/>
+      <c r="J23" s="1">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="K23" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -1429,7 +1644,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>1</v>
       </c>
@@ -1445,8 +1660,18 @@
       <c r="E26" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" s="3"/>
+      <c r="J26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>0.79727000000000003</v>
       </c>
@@ -1462,8 +1687,18 @@
       <c r="E27" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+      <c r="J27" s="1">
+        <v>0.79727000000000003</v>
+      </c>
+      <c r="K27" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>0.73</v>
       </c>
@@ -1479,8 +1714,18 @@
       <c r="E28" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" s="1"/>
+      <c r="J28" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="K28" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>0.72777999999999998</v>
       </c>
@@ -1496,8 +1741,18 @@
       <c r="E29" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" s="1"/>
+      <c r="J29" s="1">
+        <v>0.72777999999999998</v>
+      </c>
+      <c r="K29" t="s">
+        <v>6</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>0.72777999999999998</v>
       </c>
@@ -1513,8 +1768,18 @@
       <c r="E30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" s="1"/>
+      <c r="J30" s="1">
+        <v>0.72777999999999998</v>
+      </c>
+      <c r="K30" t="s">
+        <v>6</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>0.72333000000000003</v>
       </c>
@@ -1530,8 +1795,18 @@
       <c r="E31" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" s="1"/>
+      <c r="J31" s="1">
+        <v>0.72333000000000003</v>
+      </c>
+      <c r="K31" t="s">
+        <v>6</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>0.72111000000000003</v>
       </c>
@@ -1547,8 +1822,18 @@
       <c r="E32" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I32" s="1"/>
+      <c r="J32" s="1">
+        <v>0.72111000000000003</v>
+      </c>
+      <c r="K32" t="s">
+        <v>6</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>0.69333</v>
       </c>
@@ -1564,8 +1849,18 @@
       <c r="E33" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+      <c r="J33" s="1">
+        <v>0.69333</v>
+      </c>
+      <c r="K33" t="s">
+        <v>6</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>0.60111000000000003</v>
       </c>
@@ -1581,8 +1876,18 @@
       <c r="E34" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I34" s="1"/>
+      <c r="J34" s="1">
+        <v>0.60111000000000003</v>
+      </c>
+      <c r="K34" t="s">
+        <v>20</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>0.59777999999999998</v>
       </c>
@@ -1598,8 +1903,18 @@
       <c r="E35" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I35" s="1"/>
+      <c r="J35" s="1">
+        <v>0.59777999999999998</v>
+      </c>
+      <c r="K35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>0.45695000000000002</v>
       </c>
@@ -1615,8 +1930,18 @@
       <c r="E36" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I36" s="1"/>
+      <c r="J36" s="1">
+        <v>0.45695000000000002</v>
+      </c>
+      <c r="K36" t="s">
+        <v>25</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>0.43382999999999999</v>
       </c>
@@ -1632,8 +1957,18 @@
       <c r="E37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I37" s="1"/>
+      <c r="J37" s="1">
+        <v>0.43382999999999999</v>
+      </c>
+      <c r="K37" t="s">
+        <v>7</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>0.40998000000000001</v>
       </c>
@@ -1649,8 +1984,18 @@
       <c r="E38" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I38" s="1"/>
+      <c r="J38" s="1">
+        <v>0.40998000000000001</v>
+      </c>
+      <c r="K38" t="s">
+        <v>8</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>0.1133</v>
       </c>
@@ -1666,8 +2011,18 @@
       <c r="E39" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I39" s="1"/>
+      <c r="J39" s="1">
+        <v>0.1133</v>
+      </c>
+      <c r="K39" t="s">
+        <v>10</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>4.2900000000000001E-2</v>
       </c>
@@ -1682,6 +2037,16 @@
       </c>
       <c r="E40" t="b">
         <v>1</v>
+      </c>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="K40" t="s">
+        <v>9</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1695,6 +2060,486 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0.81667000000000001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.81667000000000001</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.81444000000000005</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.79727000000000003</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.81444000000000005</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.61973999999999996</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.81222000000000005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.60111000000000003</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.79727000000000003</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.52297000000000005</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.46516999999999997</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.72777999999999998</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.1133</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.72777999999999998</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.72333000000000003</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.72111000000000003</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.70667000000000002</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.69333</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.61973999999999996</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0.61602000000000001</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.61231000000000002</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0.60133999999999999</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0.60111000000000003</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0.59777999999999998</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0.52297000000000005</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0.52175000000000005</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0.51415</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>0.50927999999999995</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0.46516999999999997</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>0.45695000000000002</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>0.43382999999999999</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>0.40998000000000001</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>0.1133</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>0.1105</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>0.1099</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:C34">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C34">
+      <sortCondition descending="1" ref="A2:A34"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -1896,7 +2741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -2156,7 +3001,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Best of, All Stats
Most up to date version, albeit a bit messy
</commit_message>
<xml_diff>
--- a/stats_workbook.xlsx
+++ b/stats_workbook.xlsx
@@ -8,22 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\westw\Documents\8_2023_Spring\EENG311_Information Systems Science 2\ISSII_Group3Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{26ABB9FD-BA8F-45F6-9433-81CC5514B5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{99F33C2C-1E95-4474-8AB2-1679519346F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="21705"/>
   </bookViews>
   <sheets>
     <sheet name="stats" sheetId="1" r:id="rId1"/>
-    <sheet name="All Stats" sheetId="5" r:id="rId2"/>
-    <sheet name="LSTM Multi" sheetId="2" r:id="rId3"/>
-    <sheet name="NN_NoLSTM" sheetId="3" r:id="rId4"/>
-    <sheet name="NAR" sheetId="4" r:id="rId5"/>
+    <sheet name="Best of" sheetId="6" r:id="rId2"/>
+    <sheet name="All Stats" sheetId="5" r:id="rId3"/>
+    <sheet name="LSTM Multi" sheetId="2" r:id="rId4"/>
+    <sheet name="NN_NoLSTM" sheetId="3" r:id="rId5"/>
+    <sheet name="NAR" sheetId="4" r:id="rId6"/>
+    <sheet name="seq" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'All Stats'!$A$2:$C$34</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'LSTM Multi'!$A$2:$E$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">NAR!$A$2:$E$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">NN_NoLSTM!$A$2:$G$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'All Stats'!$A$2:$C$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Best of'!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'LSTM Multi'!$A$2:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">NAR!$A$2:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">NN_NoLSTM!$A$2:$G$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">seq!$A$1:$A$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stats!$A$26:$E$40</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="42">
   <si>
     <t>LSTM_Multichannel</t>
   </si>
@@ -142,6 +146,21 @@
   </si>
   <si>
     <t>Best of</t>
+  </si>
+  <si>
+    <t>Data Sets</t>
+  </si>
+  <si>
+    <t>Dickens</t>
+  </si>
+  <si>
+    <t>selfadapt</t>
+  </si>
+  <si>
+    <t>TrainFcn</t>
+  </si>
+  <si>
+    <t>Penalty (bits per symbol)</t>
   </si>
 </sst>
 </file>
@@ -625,7 +644,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -638,6 +657,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -997,7 +1019,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,10 +2083,139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0.61973999999999996</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0.52297000000000005</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.79727000000000003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.60111000000000003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.1133</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.81667000000000001</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.46516999999999997</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C9">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C9">
+      <sortCondition ref="C1:C9"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,17 +2246,8 @@
       <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.81667000000000001</v>
       </c>
@@ -2115,14 +2257,14 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1">
-        <v>0.81667000000000001</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>11</v>
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2136,13 +2278,13 @@
         <v>11</v>
       </c>
       <c r="F4" s="1">
-        <v>0.79727000000000003</v>
+        <v>0.81667000000000001</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2156,13 +2298,13 @@
         <v>11</v>
       </c>
       <c r="F5" s="1">
-        <v>0.61973999999999996</v>
+        <v>0.79727000000000003</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2176,13 +2318,13 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>0.60111000000000003</v>
+        <v>0.61973999999999996</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2196,13 +2338,13 @@
         <v>16</v>
       </c>
       <c r="F7" s="1">
-        <v>0.52297000000000005</v>
+        <v>0.60111000000000003</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2216,13 +2358,13 @@
         <v>16</v>
       </c>
       <c r="F8" s="1">
-        <v>0.46516999999999997</v>
+        <v>0.52297000000000005</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2236,13 +2378,13 @@
         <v>16</v>
       </c>
       <c r="F9" s="1">
-        <v>0.1133</v>
+        <v>0.46516999999999997</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2256,10 +2398,10 @@
         <v>16</v>
       </c>
       <c r="F10" s="1">
-        <v>4.2900000000000001E-2</v>
+        <v>0.1133</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>16</v>
@@ -2273,6 +2415,15 @@
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2539,7 +2690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -2741,12 +2892,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3001,12 +3152,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3043,6 +3194,12 @@
       <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -3287,4 +3444,82 @@
   <autoFilter ref="A2:E16"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A11">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A11">
+      <sortCondition ref="A1:A11"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated stats_workbook with bit penalties
</commit_message>
<xml_diff>
--- a/stats_workbook.xlsx
+++ b/stats_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\westw\Documents\8_2023_Spring\EENG311_Information Systems Science 2\ISSII_Group3Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repos\GitHub\ISSII_Group3Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{99F33C2C-1E95-4474-8AB2-1679519346F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC501F3E-8B66-4BC5-8F0A-E58518E6B0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="21705"/>
+    <workbookView xWindow="-36324" yWindow="4080" windowWidth="32244" windowHeight="18588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stats" sheetId="1" r:id="rId1"/>
@@ -28,14 +28,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">NAR!$A$2:$E$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">NN_NoLSTM!$A$2:$G$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">seq!$A$1:$A$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stats!$A$26:$E$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stats!$A$26:$E$42</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="80">
   <si>
     <t>LSTM_Multichannel</t>
   </si>
@@ -161,12 +161,592 @@
   </si>
   <si>
     <t>Penalty (bits per symbol)</t>
+  </si>
+  <si>
+    <t>Full Report Text</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 1234.561 bits (1.3717 bits per symbol).
+Correctly predicted 81.444% of symbols.
+3811 probabilities forecasted between 0% and 1%; actual occurrence rate 0.97%.
+1876 probabilities forecasted between 1% and 5%; actual occurrence rate 0.75%.
+646 probabilities forecasted between 5% and 10%; actual occurrence rate 4.18%.
+535 probabilities forecasted between 10% and 20%; actual occurrence rate 8.04%.
+188 probabilities forecasted between 20% and 30%; actual occurrence rate 13.83%.
+139 probabilities forecasted between 30% and 40%; actual occurrence rate 15.11%.
+37 probabilities forecasted between 40% and 50%; actual occurrence rate 51.35%.
+263 probabilities forecasted between 50% and 60%; actual occurrence rate 79.09%.
+129 probabilities forecasted between 60% and 70%; actual occurrence rate 78.29%.
+184 probabilities forecasted between 70% and 80%; actual occurrence rate 80.43%.
+281 probabilities forecasted between 80% and 90%; actual occurrence rate 87.54%.
+11 probabilities forecasted between 90% and 100%; actual occurrence rate 90.91%.</t>
+  </si>
+  <si>
+    <t>Total Penalty Bits</t>
+  </si>
+  <si>
+    <t>Bits per Symbol</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 5654 out of 5654 symbols in sequence_Hawaiian_test.mat.
+Total penalty: 9664.604 bits (1.7093 bits per symbol).
+Correctly predicted 61.567% of symbols.
+14496 probabilities forecasted between 0% and 1%; actual occurrence rate 0.54%.
+16101 probabilities forecasted between 1% and 5%; actual occurrence rate 1.89%.
+8013 probabilities forecasted between 5% and 10%; actual occurrence rate 6.49%.
+3506 probabilities forecasted between 10% and 20%; actual occurrence rate 16.00%.
+2815 probabilities forecasted between 20% and 30%; actual occurrence rate 20.85%.
+1479 probabilities forecasted between 30% and 40%; actual occurrence rate 33.74%.
+974 probabilities forecasted between 40% and 50%; actual occurrence rate 49.79%.
+1183 probabilities forecasted between 50% and 60%; actual occurrence rate 59.43%.
+732 probabilities forecasted between 60% and 70%; actual occurrence rate 67.49%.
+527 probabilities forecasted between 70% and 80%; actual occurrence rate 75.52%.
+403 probabilities forecasted between 80% and 90%; actual occurrence rate 93.80%.
+657 probabilities forecasted between 90% and 100%; actual occurrence rate 98.33%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 1750.950 bits (1.9455 bits per symbol).
+Correctly predicted 59.333% of symbols.
+3728 probabilities forecasted between 0% and 1%; actual occurrence rate 1.26%.
+1310 probabilities forecasted between 1% and 5%; actual occurrence rate 0.92%.
+913 probabilities forecasted between 5% and 10%; actual occurrence rate 3.72%.
+527 probabilities forecasted between 10% and 20%; actual occurrence rate 12.33%.
+453 probabilities forecasted between 20% and 30%; actual occurrence rate 23.62%.
+318 probabilities forecasted between 30% and 40%; actual occurrence rate 37.11%.
+299 probabilities forecasted between 40% and 50%; actual occurrence rate 53.51%.
+221 probabilities forecasted between 50% and 60%; actual occurrence rate 41.18%.
+137 probabilities forecasted between 60% and 70%; actual occurrence rate 75.18%.
+112 probabilities forecasted between 70% and 80%; actual occurrence rate 87.50%.
+66 probabilities forecasted between 80% and 90%; actual occurrence rate 80.30%.
+16 probabilities forecasted between 90% and 100%; actual occurrence rate 75.00%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 5654 out of 5654 symbols in sequence_Hawaiian_test.mat.
+Total penalty: 9638.105 bits (1.7047 bits per symbol).
+Correctly predicted 61.673% of symbols.
+15353 probabilities forecasted between 0% and 1%; actual occurrence rate 0.60%.
+15515 probabilities forecasted between 1% and 5%; actual occurrence rate 2.07%.
+6265 probabilities forecasted between 5% and 10%; actual occurrence rate 5.44%.
+5204 probabilities forecasted between 10% and 20%; actual occurrence rate 13.57%.
+3098 probabilities forecasted between 20% and 30%; actual occurrence rate 23.72%.
+1095 probabilities forecasted between 30% and 40%; actual occurrence rate 33.06%.
+864 probabilities forecasted between 40% and 50%; actual occurrence rate 47.34%.
+1033 probabilities forecasted between 50% and 60%; actual occurrence rate 61.96%.
+835 probabilities forecasted between 60% and 70%; actual occurrence rate 70.66%.
+481 probabilities forecasted between 70% and 80%; actual occurrence rate 75.68%.
+517 probabilities forecasted between 80% and 90%; actual occurrence rate 94.58%.
+626 probabilities forecasted between 90% and 100%; actual occurrence rate 96.65%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 5654 out of 5654 symbols in sequence_Hawaiian_test.mat.
+Total penalty: 10153.495 bits (1.7958 bits per symbol).
+Correctly predicted 61.143% of symbols.
+12327 probabilities forecasted between 0% and 1%; actual occurrence rate 1.05%.
+16741 probabilities forecasted between 1% and 5%; actual occurrence rate 1.64%.
+8153 probabilities forecasted between 5% and 10%; actual occurrence rate 4.73%.
+5925 probabilities forecasted between 10% and 20%; actual occurrence rate 13.76%.
+2195 probabilities forecasted between 20% and 30%; actual occurrence rate 25.69%.
+1366 probabilities forecasted between 30% and 40%; actual occurrence rate 34.04%.
+917 probabilities forecasted between 40% and 50%; actual occurrence rate 50.05%.
+851 probabilities forecasted between 50% and 60%; actual occurrence rate 62.51%.
+697 probabilities forecasted between 60% and 70%; actual occurrence rate 71.45%.
+683 probabilities forecasted between 70% and 80%; actual occurrence rate 81.55%.
+668 probabilities forecasted between 80% and 90%; actual occurrence rate 92.37%.
+363 probabilities forecasted between 90% and 100%; actual occurrence rate 98.62%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 3287 out of 3287 symbols in sequence_DIATemp_test.mat.
+Total penalty: 5461.353 bits (1.6615 bits per symbol).
+Correctly predicted 52.297% of symbols.
+13087 probabilities forecasted between 0% and 1%; actual occurrence rate 0.31%.
+6125 probabilities forecasted between 1% and 5%; actual occurrence rate 1.40%.
+1644 probabilities forecasted between 5% and 10%; actual occurrence rate 6.87%.
+2105 probabilities forecasted between 10% and 20%; actual occurrence rate 15.06%.
+1911 probabilities forecasted between 20% and 30%; actual occurrence rate 24.12%.
+1532 probabilities forecasted between 30% and 40%; actual occurrence rate 38.19%.
+1694 probabilities forecasted between 40% and 50%; actual occurrence rate 44.39%.
+665 probabilities forecasted between 50% and 60%; actual occurrence rate 50.38%.
+386 probabilities forecasted between 60% and 70%; actual occurrence rate 66.06%.
+434 probabilities forecasted between 70% and 80%; actual occurrence rate 79.03%.
+0 probabilities forecasted between 80% and 90%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 3287 out of 3287 symbols in sequence_DIATemp_test.mat.
+Total penalty: 5521.074 bits (1.6797 bits per symbol).
+Correctly predicted 52.297% of symbols.
+13480 probabilities forecasted between 0% and 1%; actual occurrence rate 0.27%.
+5497 probabilities forecasted between 1% and 5%; actual occurrence rate 1.67%.
+1652 probabilities forecasted between 5% and 10%; actual occurrence rate 5.51%.
+2149 probabilities forecasted between 10% and 20%; actual occurrence rate 14.43%.
+2187 probabilities forecasted between 20% and 30%; actual occurrence rate 25.15%.
+1647 probabilities forecasted between 30% and 40%; actual occurrence rate 37.77%.
+1701 probabilities forecasted between 40% and 50%; actual occurrence rate 43.92%.
+501 probabilities forecasted between 50% and 60%; actual occurrence rate 54.69%.
+345 probabilities forecasted between 60% and 70%; actual occurrence rate 65.51%.
+387 probabilities forecasted between 70% and 80%; actual occurrence rate 79.07%.
+37 probabilities forecasted between 80% and 90%; actual occurrence rate 86.49%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 10000 out of 10000 symbols in sequence_Uniform_test.mat.
+Total penalty: 32246.170 bits (3.2246 bits per symbol).
+Correctly predicted 11.390% of symbols.
+73 probabilities forecasted between 0% and 1%; actual occurrence rate 10.96%.
+1255 probabilities forecasted between 1% and 5%; actual occurrence rate 11.71%.
+29016 probabilities forecasted between 5% and 10%; actual occurrence rate 11.14%.
+59339 probabilities forecasted between 10% and 20%; actual occurrence rate 11.08%.
+310 probabilities forecasted between 20% and 30%; actual occurrence rate 11.61%.
+7 probabilities forecasted between 30% and 40%; actual occurrence rate 42.86%.
+0 probabilities forecasted between 40% and 50%.
+0 probabilities forecasted between 50% and 60%.
+0 probabilities forecasted between 60% and 70%.
+0 probabilities forecasted between 70% and 80%.
+0 probabilities forecasted between 80% and 90%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 10000 out of 10000 symbols in sequence_nonuniform_test.mat.
+Total penalty: 66471.383 bits (6.6471 bits per symbol).
+Correctly predicted 4.800% of symbols.
+26203 probabilities forecasted between 0% and 1%; actual occurrence rate 12.30%.
+14314 probabilities forecasted between 1% and 5%; actual occurrence rate 12.61%.
+18820 probabilities forecasted between 5% and 10%; actual occurrence rate 13.26%.
+11462 probabilities forecasted between 10% and 20%; actual occurrence rate 10.97%.
+5635 probabilities forecasted between 20% and 30%; actual occurrence rate 7.28%.
+8523 probabilities forecasted between 30% and 40%; actual occurrence rate 6.39%.
+5023 probabilities forecasted between 40% and 50%; actual occurrence rate 5.24%.
+20 probabilities forecasted between 50% and 60%; actual occurrence rate 0.00%.
+0 probabilities forecasted between 60% and 70%.
+0 probabilities forecasted between 70% and 80%.
+0 probabilities forecasted between 80% and 90%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 827.718 bits (0.9197 bits per symbol).
+Correctly predicted 81.667% of symbols.
+4897 probabilities forecasted between 0% and 1%; actual occurrence rate 0.04%.
+1218 probabilities forecasted between 1% and 5%; actual occurrence rate 4.35%.
+646 probabilities forecasted between 5% and 10%; actual occurrence rate 9.29%.
+440 probabilities forecasted between 10% and 20%; actual occurrence rate 11.36%.
+0 probabilities forecasted between 20% and 30%.
+3 probabilities forecasted between 30% and 40%; actual occurrence rate 66.67%.
+0 probabilities forecasted between 40% and 50%.
+0 probabilities forecasted between 50% and 60%.
+0 probabilities forecasted between 60% and 70%.
+361 probabilities forecasted between 70% and 80%; actual occurrence rate 76.45%.
+184 probabilities forecasted between 80% and 90%; actual occurrence rate 79.89%.
+351 probabilities forecasted between 90% and 100%; actual occurrence rate 88.32%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 824.943 bits (0.9166 bits per symbol).
+Correctly predicted 81.444% of symbols.
+5500 probabilities forecasted between 0% and 1%; actual occurrence rate 0.05%.
+687 probabilities forecasted between 1% and 5%; actual occurrence rate 8.15%.
+646 probabilities forecasted between 5% and 10%; actual occurrence rate 9.60%.
+368 probabilities forecasted between 10% and 20%; actual occurrence rate 12.50%.
+0 probabilities forecasted between 20% and 30%.
+0 probabilities forecasted between 30% and 40%.
+0 probabilities forecasted between 40% and 50%.
+0 probabilities forecasted between 50% and 60%.
+0 probabilities forecasted between 60% and 70%.
+303 probabilities forecasted between 70% and 80%; actual occurrence rate 77.56%.
+242 probabilities forecasted between 80% and 90%; actual occurrence rate 77.69%.
+354 probabilities forecasted between 90% and 100%; actual occurrence rate 87.57%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 824.899 bits (0.9166 bits per symbol).
+Correctly predicted 81.444% of symbols.
+5500 probabilities forecasted between 0% and 1%; actual occurrence rate 0.05%.
+687 probabilities forecasted between 1% and 5%; actual occurrence rate 8.15%.
+646 probabilities forecasted between 5% and 10%; actual occurrence rate 9.60%.
+368 probabilities forecasted between 10% and 20%; actual occurrence rate 12.50%.
+0 probabilities forecasted between 20% and 30%.
+0 probabilities forecasted between 30% and 40%.
+0 probabilities forecasted between 40% and 50%.
+0 probabilities forecasted between 50% and 60%.
+0 probabilities forecasted between 60% and 70%.
+303 probabilities forecasted between 70% and 80%; actual occurrence rate 77.56%.
+242 probabilities forecasted between 80% and 90%; actual occurrence rate 77.69%.
+354 probabilities forecasted between 90% and 100%; actual occurrence rate 87.57%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 5654 out of 5654 symbols in sequence_Hawaiian_test.mat.
+Total penalty: 10093.810 bits (1.7853 bits per symbol).
+Correctly predicted 60.134% of symbols.
+13139 probabilities forecasted between 0% and 1%; actual occurrence rate 0.58%.
+15809 probabilities forecasted between 1% and 5%; actual occurrence rate 2.14%.
+11598 probabilities forecasted between 5% and 10%; actual occurrence rate 6.77%.
+152 probabilities forecasted between 10% and 20%; actual occurrence rate 13.16%.
+4534 probabilities forecasted between 20% and 30%; actual occurrence rate 22.81%.
+0 probabilities forecasted between 30% and 40%.
+2401 probabilities forecasted between 40% and 50%; actual occurrence rate 46.36%.
+2089 probabilities forecasted between 50% and 60%; actual occurrence rate 57.83%.
+0 probabilities forecasted between 60% and 70%.
+44 probabilities forecasted between 70% and 80%; actual occurrence rate 50.00%.
+152 probabilities forecasted between 80% and 90%; actual occurrence rate 85.53%.
+968 probabilities forecasted between 90% and 100%; actual occurrence rate 95.76%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 3287 out of 3287 symbols in sequence_DIAtemp_test.mat.
+Total penalty: 5638.267 bits (1.7153 bits per symbol).
+Correctly predicted 50.928% of symbols.
+15591 probabilities forecasted between 0% and 1%; actual occurrence rate 0.26%.
+2769 probabilities forecasted between 1% and 5%; actual occurrence rate 2.67%.
+2026 probabilities forecasted between 5% and 10%; actual occurrence rate 5.38%.
+2006 probabilities forecasted between 10% and 20%; actual occurrence rate 18.25%.
+2748 probabilities forecasted between 20% and 30%; actual occurrence rate 21.83%.
+1530 probabilities forecasted between 30% and 40%; actual occurrence rate 36.80%.
+1535 probabilities forecasted between 40% and 50%; actual occurrence rate 42.41%.
+729 probabilities forecasted between 50% and 60%; actual occurrence rate 55.14%.
+0 probabilities forecasted between 60% and 70%.
+649 probabilities forecasted between 70% and 80%; actual occurrence rate 74.27%.
+0 probabilities forecasted between 80% and 90%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 3287 out of 3287 symbols in sequence_DIAtemp_test.mat.
+Total penalty: 5618.304 bits (1.7092 bits per symbol).
+Correctly predicted 50.928% of symbols.
+13593 probabilities forecasted between 0% and 1%; actual occurrence rate 0.24%.
+4938 probabilities forecasted between 1% and 5%; actual occurrence rate 1.74%.
+1841 probabilities forecasted between 5% and 10%; actual occurrence rate 5.54%.
+1263 probabilities forecasted between 10% and 20%; actual occurrence rate 16.15%.
+3473 probabilities forecasted between 20% and 30%; actual occurrence rate 21.80%.
+1208 probabilities forecasted between 30% and 40%; actual occurrence rate 36.34%.
+1898 probabilities forecasted between 40% and 50%; actual occurrence rate 41.57%.
+720 probabilities forecasted between 50% and 60%; actual occurrence rate 54.86%.
+0 probabilities forecasted between 60% and 70%.
+649 probabilities forecasted between 70% and 80%; actual occurrence rate 74.27%.
+0 probabilities forecasted between 80% and 90%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Not sure how this was set up, feel free to rerun and put in all the data</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 10000 out of 10000 symbols in sequence_uniform_test.mat.
+Total penalty: 31763.324 bits (3.1763 bits per symbol).
+Correctly predicted 11.460% of symbols.
+0 probabilities forecasted between 0% and 1%.
+0 probabilities forecasted between 1% and 5%.
+16687 probabilities forecasted between 5% and 10%; actual occurrence rate 11.07%.
+73313 probabilities forecasted between 10% and 20%; actual occurrence rate 11.12%.
+0 probabilities forecasted between 20% and 30%.
+0 probabilities forecasted between 30% and 40%.
+0 probabilities forecasted between 40% and 50%.
+0 probabilities forecasted between 50% and 60%.
+0 probabilities forecasted between 60% and 70%.
+0 probabilities forecasted between 70% and 80%.
+0 probabilities forecasted between 80% and 90%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 10000 out of 10000 symbols in sequence_nonuniform_test.mat.
+Total penalty: 32561.621 bits (3.2562 bits per symbol).
+Correctly predicted 2.190% of symbols.
+0 probabilities forecasted between 0% and 1%.
+20000 probabilities forecasted between 1% and 5%; actual occurrence rate 3.29%.
+20000 probabilities forecasted between 5% and 10%; actual occurrence rate 13.12%.
+44377 probabilities forecasted between 10% and 20%; actual occurrence rate 14.87%.
+5623 probabilities forecasted between 20% and 30%; actual occurrence rate 2.12%.
+0 probabilities forecasted between 30% and 40%.
+0 probabilities forecasted between 40% and 50%.
+0 probabilities forecasted between 50% and 60%.
+0 probabilities forecasted between 60% and 70%.
+0 probabilities forecasted between 70% and 80%.
+0 probabilities forecasted between 80% and 90%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 952 out of 952 symbols in sequence_solarWind_test.mat.
+Total penalty: 951.064 bits (0.9990 bits per symbol).
+Correctly predicted 79.097% of symbols.
+4793 probabilities forecasted between 0% and 1%; actual occurrence rate 0.31%.
+1297 probabilities forecasted between 1% and 5%; actual occurrence rate 1.00%.
+1084 probabilities forecasted between 5% and 10%; actual occurrence rate 7.56%.
+285 probabilities forecasted between 10% and 20%; actual occurrence rate 14.74%.
+115 probabilities forecasted between 20% and 30%; actual occurrence rate 23.48%.
+12 probabilities forecasted between 30% and 40%; actual occurrence rate 41.67%.
+71 probabilities forecasted between 40% and 50%; actual occurrence rate 43.66%.
+4 probabilities forecasted between 50% and 60%; actual occurrence rate 75.00%.
+110 probabilities forecasted between 60% and 70%; actual occurrence rate 70.00%.
+33 probabilities forecasted between 70% and 80%; actual occurrence rate 60.61%.
+764 probabilities forecasted between 80% and 90%; actual occurrence rate 83.38%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 1353.373 bits (1.5037 bits per symbol).
+Correctly predicted 72.889% of symbols.
+5692 probabilities forecasted between 0% and 1%; actual occurrence rate 0.84%.
+299 probabilities forecasted between 1% and 5%; actual occurrence rate 8.03%.
+849 probabilities forecasted between 5% and 10%; actual occurrence rate 11.54%.
+320 probabilities forecasted between 10% and 20%; actual occurrence rate 19.38%.
+19 probabilities forecasted between 20% and 30%; actual occurrence rate 31.58%.
+6 probabilities forecasted between 30% and 40%; actual occurrence rate 33.33%.
+19 probabilities forecasted between 40% and 50%; actual occurrence rate 21.05%.
+20 probabilities forecasted between 50% and 60%; actual occurrence rate 65.00%.
+3 probabilities forecasted between 60% and 70%; actual occurrence rate 0.00%.
+95 probabilities forecasted between 70% and 80%; actual occurrence rate 71.58%.
+374 probabilities forecasted between 80% and 90%; actual occurrence rate 69.52%.
+404 probabilities forecasted between 90% and 100%; actual occurrence rate 77.97%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 1541.812 bits (1.7131 bits per symbol).
+Correctly predicted 72.778% of symbols.
+5747 probabilities forecasted between 0% and 1%; actual occurrence rate 0.96%.
+260 probabilities forecasted between 1% and 5%; actual occurrence rate 7.69%.
+994 probabilities forecasted between 5% and 10%; actual occurrence rate 12.17%.
+162 probabilities forecasted between 10% and 20%; actual occurrence rate 23.46%.
+22 probabilities forecasted between 20% and 30%; actual occurrence rate 31.82%.
+1 probabilities forecasted between 30% and 40%; actual occurrence rate 0.00%.
+18 probabilities forecasted between 40% and 50%; actual occurrence rate 22.22%.
+17 probabilities forecasted between 50% and 60%; actual occurrence rate 58.82%.
+0 probabilities forecasted between 60% and 70%.
+96 probabilities forecasted between 70% and 80%; actual occurrence rate 70.83%.
+592 probabilities forecasted between 80% and 90%; actual occurrence rate 74.49%.
+191 probabilities forecasted between 90% and 100%; actual occurrence rate 71.20%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 1682.832 bits (1.8698 bits per symbol).
+Correctly predicted 73.000% of symbols.
+2631 probabilities forecasted between 0% and 1%; actual occurrence rate 0.11%.
+1288 probabilities forecasted between 1% and 5%; actual occurrence rate 0.08%.
+237 probabilities forecasted between 5% and 10%; actual occurrence rate 0.00%.
+1423 probabilities forecasted between 10% and 20%; actual occurrence rate 1.05%.
+2066 probabilities forecasted between 20% and 30%; actual occurrence rate 28.07%.
+351 probabilities forecasted between 30% and 40%; actual occurrence rate 62.96%.
+103 probabilities forecasted between 40% and 50%; actual occurrence rate 77.67%.
+0 probabilities forecasted between 50% and 60%.
+1 probabilities forecasted between 60% and 70%; actual occurrence rate 0.00%.
+0 probabilities forecasted between 70% and 80%.
+0 probabilities forecasted between 80% and 90%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 1097.593 bits (1.2195 bits per symbol).
+Correctly predicted 72.000% of symbols.
+5486 probabilities forecasted between 0% and 1%; actual occurrence rate 0.27%.
+49 probabilities forecasted between 1% and 5%; actual occurrence rate 0.00%.
+526 probabilities forecasted between 5% and 10%; actual occurrence rate 9.70%.
+1094 probabilities forecasted between 10% and 20%; actual occurrence rate 14.99%.
+18 probabilities forecasted between 20% and 30%; actual occurrence rate 38.89%.
+13 probabilities forecasted between 30% and 40%; actual occurrence rate 38.46%.
+17 probabilities forecasted between 40% and 50%; actual occurrence rate 58.82%.
+17 probabilities forecasted between 50% and 60%; actual occurrence rate 23.53%.
+13 probabilities forecasted between 60% and 70%; actual occurrence rate 61.54%.
+764 probabilities forecasted between 70% and 80%; actual occurrence rate 72.77%.
+101 probabilities forecasted between 80% and 90%; actual occurrence rate 79.21%.
+2 probabilities forecasted between 90% and 100%; actual occurrence rate 0.00%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 1668.934 bits (1.8544 bits per symbol).
+Correctly predicted 72.222% of symbols.
+2662 probabilities forecasted between 0% and 1%; actual occurrence rate 0.00%.
+1262 probabilities forecasted between 1% and 5%; actual occurrence rate 0.08%.
+178 probabilities forecasted between 5% and 10%; actual occurrence rate 1.12%.
+1454 probabilities forecasted between 10% and 20%; actual occurrence rate 1.24%.
+2110 probabilities forecasted between 20% and 30%; actual occurrence rate 27.87%.
+333 probabilities forecasted between 30% and 40%; actual occurrence rate 63.36%.
+101 probabilities forecasted between 40% and 50%; actual occurrence rate 79.21%.
+0 probabilities forecasted between 50% and 60%.
+0 probabilities forecasted between 60% and 70%.
+0 probabilities forecasted between 70% and 80%.
+0 probabilities forecasted between 80% and 90%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>hear2</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 1188.988 bits (1.3211 bits per symbol).
+Correctly predicted 72.889% of symbols.
+5537 probabilities forecasted between 0% and 1%; actual occurrence rate 0.45%.
+348 probabilities forecasted between 1% and 5%; actual occurrence rate 10.06%.
+408 probabilities forecasted between 5% and 10%; actual occurrence rate 10.05%.
+508 probabilities forecasted between 10% and 20%; actual occurrence rate 13.58%.
+148 probabilities forecasted between 20% and 30%; actual occurrence rate 21.62%.
+211 probabilities forecasted between 30% and 40%; actual occurrence rate 18.96%.
+82 probabilities forecasted between 40% and 50%; actual occurrence rate 37.80%.
+17 probabilities forecasted between 50% and 60%; actual occurrence rate 58.82%.
+272 probabilities forecasted between 60% and 70%; actual occurrence rate 68.01%.
+479 probabilities forecasted between 70% and 80%; actual occurrence rate 75.16%.
+89 probabilities forecasted between 80% and 90%; actual occurrence rate 80.90%.
+1 probabilities forecasted between 90% and 100%; actual occurrence rate 0.00%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 1419.881 bits (1.5776 bits per symbol).
+Correctly predicted 73.000% of symbols.
+5712 probabilities forecasted between 0% and 1%; actual occurrence rate 0.77%.
+566 probabilities forecasted between 1% and 5%; actual occurrence rate 7.77%.
+717 probabilities forecasted between 5% and 10%; actual occurrence rate 14.37%.
+159 probabilities forecasted between 10% and 20%; actual occurrence rate 23.27%.
+17 probabilities forecasted between 20% and 30%; actual occurrence rate 35.29%.
+13 probabilities forecasted between 30% and 40%; actual occurrence rate 38.46%.
+17 probabilities forecasted between 40% and 50%; actual occurrence rate 23.53%.
+17 probabilities forecasted between 50% and 60%; actual occurrence rate 58.82%.
+15 probabilities forecasted between 60% and 70%; actual occurrence rate 53.33%.
+136 probabilities forecasted between 70% and 80%; actual occurrence rate 71.32%.
+349 probabilities forecasted between 80% and 90%; actual occurrence rate 69.91%.
+382 probabilities forecasted between 90% and 100%; actual occurrence rate 78.01%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart2_test.mat.
+Total penalty: 1730.141 bits (1.9224 bits per symbol).
+Correctly predicted 69.556% of symbols.
+4149 probabilities forecasted between 0% and 1%; actual occurrence rate 1.37%.
+1361 probabilities forecasted between 1% and 5%; actual occurrence rate 2.35%.
+771 probabilities forecasted between 5% and 10%; actual occurrence rate 7.00%.
+641 probabilities forecasted between 10% and 20%; actual occurrence rate 11.39%.
+217 probabilities forecasted between 20% and 30%; actual occurrence rate 19.82%.
+79 probabilities forecasted between 30% and 40%; actual occurrence rate 24.05%.
+74 probabilities forecasted between 40% and 50%; actual occurrence rate 44.59%.
+82 probabilities forecasted between 50% and 60%; actual occurrence rate 62.20%.
+127 probabilities forecasted between 60% and 70%; actual occurrence rate 66.14%.
+321 probabilities forecasted between 70% and 80%; actual occurrence rate 71.65%.
+266 probabilities forecasted between 80% and 90%; actual occurrence rate 80.08%.
+12 probabilities forecasted between 90% and 100%; actual occurrence rate 91.67%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart1_test.mat.
+Total penalty: 1726.552 bits (1.9184 bits per symbol).
+Correctly predicted 60.111% of symbols.
+5204 probabilities forecasted between 0% and 1%; actual occurrence rate 0.88%.
+527 probabilities forecasted between 1% and 5%; actual occurrence rate 6.45%.
+618 probabilities forecasted between 5% and 10%; actual occurrence rate 14.08%.
+666 probabilities forecasted between 10% and 20%; actual occurrence rate 18.47%.
+132 probabilities forecasted between 20% and 30%; actual occurrence rate 28.79%.
+63 probabilities forecasted between 30% and 40%; actual occurrence rate 57.14%.
+5 probabilities forecasted between 40% and 50%; actual occurrence rate 60.00%.
+2 probabilities forecasted between 50% and 60%; actual occurrence rate 0.00%.
+69 probabilities forecasted between 60% and 70%; actual occurrence rate 31.88%.
+443 probabilities forecasted between 70% and 80%; actual occurrence rate 64.79%.
+335 probabilities forecasted between 80% and 90%; actual occurrence rate 60.60%.
+36 probabilities forecasted between 90% and 100%; actual occurrence rate 58.33%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart1_test.mat.
+Total penalty: 1706.893 bits (1.8965 bits per symbol).
+Correctly predicted 59.667% of symbols.
+4423 probabilities forecasted between 0% and 1%; actual occurrence rate 0.66%.
+1152 probabilities forecasted between 1% and 5%; actual occurrence rate 3.99%.
+639 probabilities forecasted between 5% and 10%; actual occurrence rate 12.99%.
+785 probabilities forecasted between 10% and 20%; actual occurrence rate 20.38%.
+198 probabilities forecasted between 20% and 30%; actual occurrence rate 22.73%.
+11 probabilities forecasted between 30% and 40%; actual occurrence rate 9.09%.
+43 probabilities forecasted between 40% and 50%; actual occurrence rate 25.58%.
+38 probabilities forecasted between 50% and 60%; actual occurrence rate 68.42%.
+188 probabilities forecasted between 60% and 70%; actual occurrence rate 68.09%.
+330 probabilities forecasted between 70% and 80%; actual occurrence rate 58.18%.
+293 probabilities forecasted between 80% and 90%; actual occurrence rate 61.09%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 3287 out of 3287 symbols in sequence_DIAwind_test.mat.
+Total penalty: 6451.225 bits (1.9626 bits per symbol).
+Correctly predicted 45.634% of symbols.
+12115 probabilities forecasted between 0% and 1%; actual occurrence rate 0.36%.
+4665 probabilities forecasted between 1% and 5%; actual occurrence rate 2.55%.
+3572 probabilities forecasted between 5% and 10%; actual occurrence rate 8.79%.
+2414 probabilities forecasted between 10% and 20%; actual occurrence rate 10.69%.
+2127 probabilities forecasted between 20% and 30%; actual occurrence rate 28.30%.
+1957 probabilities forecasted between 30% and 40%; actual occurrence rate 33.42%.
+1746 probabilities forecasted between 40% and 50%; actual occurrence rate 46.62%.
+987 probabilities forecasted between 50% and 60%; actual occurrence rate 48.83%.
+0 probabilities forecasted between 60% and 70%.
+0 probabilities forecasted between 70% and 80%.
+0 probabilities forecasted between 80% and 90%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 3287 out of 3287 symbols in sequence_DIAtemp_test.mat.
+Total penalty: 6758.492 bits (2.0561 bits per symbol).
+Correctly predicted 43.353% of symbols.
+15001 probabilities forecasted between 0% and 1%; actual occurrence rate 0.65%.
+3691 probabilities forecasted between 1% and 5%; actual occurrence rate 5.07%.
+1922 probabilities forecasted between 5% and 10%; actual occurrence rate 9.16%.
+1634 probabilities forecasted between 10% and 20%; actual occurrence rate 16.34%.
+2822 probabilities forecasted between 20% and 30%; actual occurrence rate 24.98%.
+1656 probabilities forecasted between 30% and 40%; actual occurrence rate 36.23%.
+1463 probabilities forecasted between 40% and 50%; actual occurrence rate 34.31%.
+748 probabilities forecasted between 50% and 60%; actual occurrence rate 42.78%.
+157 probabilities forecasted between 60% and 70%; actual occurrence rate 62.42%.
+482 probabilities forecasted between 70% and 80%; actual occurrence rate 68.26%.
+7 probabilities forecasted between 80% and 90%; actual occurrence rate 85.71%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 5654 out of 5654 symbols in sequence_Hawaiian_test.mat.
+Total penalty: 17432.941 bits (3.0833 bits per symbol).
+Correctly predicted 41.051% of symbols.
+16083 probabilities forecasted between 0% and 1%; actual occurrence rate 4.46%.
+17087 probabilities forecasted between 1% and 5%; actual occurrence rate 3.96%.
+5637 probabilities forecasted between 5% and 10%; actual occurrence rate 4.24%.
+2887 probabilities forecasted between 10% and 20%; actual occurrence rate 20.57%.
+4381 probabilities forecasted between 20% and 30%; actual occurrence rate 38.01%.
+431 probabilities forecasted between 30% and 40%; actual occurrence rate 31.79%.
+558 probabilities forecasted between 40% and 50%; actual occurrence rate 33.15%.
+893 probabilities forecasted between 50% and 60%; actual occurrence rate 23.07%.
+1537 probabilities forecasted between 60% and 70%; actual occurrence rate 55.11%.
+235 probabilities forecasted between 70% and 80%; actual occurrence rate 37.45%.
+247 probabilities forecasted between 80% and 90%; actual occurrence rate 18.22%.
+910 probabilities forecasted between 90% and 100%; actual occurrence rate 27.91%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 10000 out of 10000 symbols in sequence_uniform_test.mat.
+Total penalty: 32117.952 bits (3.2118 bits per symbol).
+Correctly predicted 11.160% of symbols.
+4 probabilities forecasted between 0% and 1%; actual occurrence rate 25.00%.
+324 probabilities forecasted between 1% and 5%; actual occurrence rate 11.73%.
+27739 probabilities forecasted between 5% and 10%; actual occurrence rate 11.40%.
+61930 probabilities forecasted between 10% and 20%; actual occurrence rate 10.98%.
+2 probabilities forecasted between 20% and 30%; actual occurrence rate 0.00%.
+1 probabilities forecasted between 30% and 40%; actual occurrence rate 0.00%.
+0 probabilities forecasted between 40% and 50%.
+0 probabilities forecasted between 50% and 60%.
+0 probabilities forecasted between 60% and 70%.
+0 probabilities forecasted between 70% and 80%.
+0 probabilities forecasted between 80% and 90%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 10000 out of 10000 symbols in sequence_nonuniform_test.mat.
+Total penalty: 32641.158 bits (3.2641 bits per symbol).
+Correctly predicted 3.030% of symbols.
+35 probabilities forecasted between 0% and 1%; actual occurrence rate 0.00%.
+14730 probabilities forecasted between 1% and 5%; actual occurrence rate 3.41%.
+23954 probabilities forecasted between 5% and 10%; actual occurrence rate 11.58%.
+48177 probabilities forecasted between 10% and 20%; actual occurrence rate 13.76%.
+3104 probabilities forecasted between 20% and 30%; actual occurrence rate 3.06%.
+0 probabilities forecasted between 30% and 40%.
+0 probabilities forecasted between 40% and 50%.
+0 probabilities forecasted between 50% and 60%.
+0 probabilities forecasted between 60% and 70%.
+0 probabilities forecasted between 70% and 80%.
+0 probabilities forecasted between 80% and 90%.
+0 probabilities forecasted between 90% and 100%.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -303,7 +883,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,6 +1063,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -644,14 +1230,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -661,6 +1246,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1015,28 +1623,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5546875" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="89.109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1045,10 +1655,8 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1061,7 +1669,12 @@
       <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="J2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1071,11 +1684,12 @@
       <c r="L2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>0.81222000000000005</v>
-      </c>
+      <c r="M2" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -1088,9 +1702,14 @@
       <c r="E3">
         <v>40</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1">
-        <v>0.81222000000000005</v>
+      <c r="H3">
+        <v>1234.5609999999999</v>
+      </c>
+      <c r="I3" s="12">
+        <v>1.3716999999999999</v>
+      </c>
+      <c r="J3" s="14">
+        <v>0.81444000000000005</v>
       </c>
       <c r="K3" t="s">
         <v>6</v>
@@ -1098,11 +1717,12 @@
       <c r="L3" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0.70667000000000002</v>
-      </c>
+      <c r="M3" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -1115,9 +1735,14 @@
       <c r="E4">
         <v>40</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1">
-        <v>0.70667000000000002</v>
+      <c r="H4">
+        <v>1750.95</v>
+      </c>
+      <c r="I4" s="12">
+        <v>1.9455</v>
+      </c>
+      <c r="J4" s="14">
+        <v>0.59333000000000002</v>
       </c>
       <c r="K4" t="s">
         <v>6</v>
@@ -1125,11 +1750,12 @@
       <c r="L4" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.61973999999999996</v>
-      </c>
+      <c r="M4" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -1142,9 +1768,14 @@
       <c r="E5">
         <v>150</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1">
-        <v>0.61973999999999996</v>
+      <c r="H5">
+        <v>9664.6039999999994</v>
+      </c>
+      <c r="I5" s="12">
+        <v>1.7093</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0.61567000000000005</v>
       </c>
       <c r="K5" t="s">
         <v>8</v>
@@ -1152,11 +1783,12 @@
       <c r="L5" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.61602000000000001</v>
-      </c>
+      <c r="M5" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -1169,9 +1801,14 @@
       <c r="E6">
         <v>40</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1">
-        <v>0.61602000000000001</v>
+      <c r="H6">
+        <v>9638.1049999999996</v>
+      </c>
+      <c r="I6" s="12">
+        <v>1.7074</v>
+      </c>
+      <c r="J6" s="14">
+        <v>0.61673</v>
       </c>
       <c r="K6" t="s">
         <v>8</v>
@@ -1179,11 +1816,12 @@
       <c r="L6" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.61231000000000002</v>
-      </c>
+      <c r="M6" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -1196,9 +1834,14 @@
       <c r="E7">
         <v>40</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1">
-        <v>0.61231000000000002</v>
+      <c r="H7">
+        <v>10153.495000000001</v>
+      </c>
+      <c r="I7" s="12">
+        <v>1.7958000000000001</v>
+      </c>
+      <c r="J7" s="14">
+        <v>0.61143000000000003</v>
       </c>
       <c r="K7" t="s">
         <v>8</v>
@@ -1206,11 +1849,12 @@
       <c r="L7" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.52297000000000005</v>
-      </c>
+      <c r="M7" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -1223,8 +1867,13 @@
       <c r="E8">
         <v>40</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1">
+      <c r="H8">
+        <v>5461.3530000000001</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1.6615</v>
+      </c>
+      <c r="J8" s="14">
         <v>0.52297000000000005</v>
       </c>
       <c r="K8" t="s">
@@ -1233,11 +1882,12 @@
       <c r="L8" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.52175000000000005</v>
-      </c>
+      <c r="M8" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -1250,9 +1900,14 @@
       <c r="E9">
         <v>40</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1">
-        <v>0.52175000000000005</v>
+      <c r="H9">
+        <v>5521.0739999999996</v>
+      </c>
+      <c r="I9" s="12">
+        <v>1.6797</v>
+      </c>
+      <c r="J9" s="14">
+        <v>0.52297000000000005</v>
       </c>
       <c r="K9" t="s">
         <v>7</v>
@@ -1260,11 +1915,12 @@
       <c r="L9" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.1099</v>
-      </c>
+      <c r="M9" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -1277,9 +1933,14 @@
       <c r="E10">
         <v>150</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1">
-        <v>0.1099</v>
+      <c r="H10">
+        <v>32246.17</v>
+      </c>
+      <c r="I10" s="12">
+        <v>3.2246000000000001</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0.1139</v>
       </c>
       <c r="K10" t="s">
         <v>10</v>
@@ -1287,11 +1948,12 @@
       <c r="L10" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>3.4299999999999997E-2</v>
-      </c>
+      <c r="M10" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -1304,9 +1966,14 @@
       <c r="E11">
         <v>150</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1">
-        <v>3.4299999999999997E-2</v>
+      <c r="H11">
+        <v>66471.383000000002</v>
+      </c>
+      <c r="I11" s="12">
+        <v>6.6471</v>
+      </c>
+      <c r="J11" s="14">
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="K11" t="s">
         <v>9</v>
@@ -1314,8 +1981,14 @@
       <c r="L11" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1323,11 +1996,10 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1346,8 +2018,13 @@
       <c r="G14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3" t="s">
+      <c r="H14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="15" t="s">
         <v>1</v>
       </c>
       <c r="K14" s="3" t="s">
@@ -1357,10 +2034,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.81667000000000001</v>
-      </c>
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>6</v>
       </c>
@@ -1373,14 +2048,19 @@
       <c r="E15">
         <v>40</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1">
+      <c r="H15">
+        <v>827.71799999999996</v>
+      </c>
+      <c r="I15" s="12">
+        <v>0.91969999999999996</v>
+      </c>
+      <c r="J15" s="14">
         <v>0.81667000000000001</v>
       </c>
       <c r="K15" t="s">
@@ -1389,11 +2069,12 @@
       <c r="L15" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>0.81444000000000005</v>
-      </c>
+      <c r="M15" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>6</v>
       </c>
@@ -1406,14 +2087,19 @@
       <c r="E16">
         <v>40</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1">
+      <c r="H16">
+        <v>824.94299999999998</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0.91659999999999997</v>
+      </c>
+      <c r="J16" s="14">
         <v>0.81444000000000005</v>
       </c>
       <c r="K16" t="s">
@@ -1422,11 +2108,12 @@
       <c r="L16" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0.81444000000000005</v>
-      </c>
+      <c r="M16" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -1439,14 +2126,19 @@
       <c r="E17">
         <v>40</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1">
+      <c r="H17">
+        <v>824.899</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0.91659999999999997</v>
+      </c>
+      <c r="J17" s="14">
         <v>0.81444000000000005</v>
       </c>
       <c r="K17" t="s">
@@ -1455,11 +2147,12 @@
       <c r="L17" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0.60133999999999999</v>
-      </c>
+      <c r="M17" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -1472,14 +2165,19 @@
       <c r="E18">
         <v>40</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1">
+      <c r="H18">
+        <v>10093.81</v>
+      </c>
+      <c r="I18" s="12">
+        <v>1.7853000000000001</v>
+      </c>
+      <c r="J18" s="14">
         <v>0.60133999999999999</v>
       </c>
       <c r="K18" t="s">
@@ -1488,11 +2186,12 @@
       <c r="L18" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.51415</v>
-      </c>
+      <c r="M18" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
       <c r="B19" t="s">
         <v>7</v>
       </c>
@@ -1505,15 +2204,20 @@
       <c r="E19">
         <v>40</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1">
-        <v>0.51415</v>
+      <c r="H19">
+        <v>5638.2669999999998</v>
+      </c>
+      <c r="I19" s="12">
+        <v>1.7153</v>
+      </c>
+      <c r="J19" s="14">
+        <v>0.50927999999999995</v>
       </c>
       <c r="K19" t="s">
         <v>7</v>
@@ -1521,11 +2225,12 @@
       <c r="L19" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>0.50927999999999995</v>
-      </c>
+      <c r="M19" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -1538,14 +2243,19 @@
       <c r="E20">
         <v>40</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1">
+      <c r="H20">
+        <v>5618.3040000000001</v>
+      </c>
+      <c r="I20" s="12">
+        <v>1.7092000000000001</v>
+      </c>
+      <c r="J20" s="14">
         <v>0.50927999999999995</v>
       </c>
       <c r="K20" t="s">
@@ -1554,44 +2264,46 @@
       <c r="L20" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="M20" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="8">
+        <v>40</v>
+      </c>
+      <c r="F21" s="16">
+        <v>1</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="17"/>
+      <c r="J21" s="18">
         <v>0.46516999999999997</v>
       </c>
-      <c r="B21" t="s">
+      <c r="K21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21">
-        <v>40</v>
-      </c>
-      <c r="F21" s="5">
-        <v>1</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1">
-        <v>0.46516999999999997</v>
-      </c>
-      <c r="K21" t="s">
-        <v>25</v>
-      </c>
-      <c r="L21" s="3" t="s">
+      <c r="L21" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>0.1105</v>
-      </c>
+      <c r="M21" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
       <c r="B22" t="s">
         <v>10</v>
       </c>
@@ -1604,15 +2316,20 @@
       <c r="E22">
         <v>40</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1">
-        <v>0.1105</v>
+      <c r="H22">
+        <v>31763.324000000001</v>
+      </c>
+      <c r="I22" s="12">
+        <v>3.1762999999999999</v>
+      </c>
+      <c r="J22" s="14">
+        <v>0.11459999999999999</v>
       </c>
       <c r="K22" t="s">
         <v>10</v>
@@ -1620,11 +2337,12 @@
       <c r="L22" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>2.5399999999999999E-2</v>
-      </c>
+      <c r="M22" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
       <c r="B23" t="s">
         <v>9</v>
       </c>
@@ -1637,15 +2355,20 @@
       <c r="E23">
         <v>40</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1">
-        <v>2.5399999999999999E-2</v>
+      <c r="H23">
+        <v>32561.620999999999</v>
+      </c>
+      <c r="I23" s="12">
+        <v>3.2562000000000002</v>
+      </c>
+      <c r="J23" s="14">
+        <v>2.1899999999999999E-2</v>
       </c>
       <c r="K23" t="s">
         <v>9</v>
@@ -1653,11 +2376,15 @@
       <c r="L23" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -1665,11 +2392,10 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
@@ -1682,8 +2408,13 @@
       <c r="E26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3" t="s">
+      <c r="H26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="15" t="s">
         <v>1</v>
       </c>
       <c r="K26" s="3" t="s">
@@ -1693,10 +2424,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>0.79727000000000003</v>
-      </c>
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -1709,9 +2438,14 @@
       <c r="E27" t="b">
         <v>1</v>
       </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1">
-        <v>0.79727000000000003</v>
+      <c r="H27">
+        <v>951.06399999999996</v>
+      </c>
+      <c r="I27" s="12">
+        <v>0.999</v>
+      </c>
+      <c r="J27" s="14">
+        <v>0.79096999999999995</v>
       </c>
       <c r="K27" t="s">
         <v>26</v>
@@ -1719,11 +2453,12 @@
       <c r="L27" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>0.73</v>
-      </c>
+      <c r="M27" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
       <c r="B28" t="s">
         <v>6</v>
       </c>
@@ -1736,9 +2471,14 @@
       <c r="E28" t="b">
         <v>1</v>
       </c>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1">
-        <v>0.73</v>
+      <c r="H28">
+        <v>1353.373</v>
+      </c>
+      <c r="I28" s="12">
+        <v>1.5037</v>
+      </c>
+      <c r="J28" s="14">
+        <v>0.72889000000000004</v>
       </c>
       <c r="K28" t="s">
         <v>6</v>
@@ -1746,11 +2486,12 @@
       <c r="L28" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>0.72777999999999998</v>
-      </c>
+      <c r="M28" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
       <c r="B29" t="s">
         <v>6</v>
       </c>
@@ -1763,8 +2504,13 @@
       <c r="E29" t="b">
         <v>1</v>
       </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1">
+      <c r="H29">
+        <v>1541.8119999999999</v>
+      </c>
+      <c r="I29" s="12">
+        <v>1.7131000000000001</v>
+      </c>
+      <c r="J29" s="14">
         <v>0.72777999999999998</v>
       </c>
       <c r="K29" t="s">
@@ -1773,11 +2519,12 @@
       <c r="L29" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>0.72777999999999998</v>
-      </c>
+      <c r="M29" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
       <c r="B30" t="s">
         <v>6</v>
       </c>
@@ -1785,14 +2532,19 @@
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E30" t="s">
         <v>28</v>
       </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1">
-        <v>0.72777999999999998</v>
+      <c r="H30">
+        <v>1682.8320000000001</v>
+      </c>
+      <c r="I30" s="12">
+        <v>1.8697999999999999</v>
+      </c>
+      <c r="J30" s="14">
+        <v>0.73</v>
       </c>
       <c r="K30" t="s">
         <v>6</v>
@@ -1800,11 +2552,12 @@
       <c r="L30" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>0.72333000000000003</v>
-      </c>
+      <c r="M30" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
       <c r="B31" t="s">
         <v>6</v>
       </c>
@@ -1815,11 +2568,16 @@
         <v>21</v>
       </c>
       <c r="E31" t="s">
-        <v>27</v>
-      </c>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1">
-        <v>0.72333000000000003</v>
+        <v>28</v>
+      </c>
+      <c r="H31">
+        <v>1668.934</v>
+      </c>
+      <c r="I31" s="12">
+        <v>1.8544</v>
+      </c>
+      <c r="J31" s="14">
+        <v>0.72221999999999997</v>
       </c>
       <c r="K31" t="s">
         <v>6</v>
@@ -1827,26 +2585,32 @@
       <c r="L31" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>0.72111000000000003</v>
-      </c>
+      <c r="M31" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="C32" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1">
-        <v>0.72111000000000003</v>
+        <v>21</v>
+      </c>
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32">
+        <v>1188.9880000000001</v>
+      </c>
+      <c r="I32" s="12">
+        <v>1.3210999999999999</v>
+      </c>
+      <c r="J32" s="14">
+        <v>0.72889000000000004</v>
       </c>
       <c r="K32" t="s">
         <v>6</v>
@@ -1854,26 +2618,32 @@
       <c r="L32" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>0.69333</v>
-      </c>
+      <c r="M32" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
       <c r="B33" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="2">
-        <v>4.8611111111111112E-2</v>
+        <v>4.3055555555555562E-2</v>
       </c>
       <c r="D33" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" t="b">
-        <v>1</v>
-      </c>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1">
-        <v>0.69333</v>
+        <v>24</v>
+      </c>
+      <c r="E33" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33">
+        <v>1097.5930000000001</v>
+      </c>
+      <c r="I33" s="12">
+        <v>1.2195</v>
+      </c>
+      <c r="J33" s="14">
+        <v>0.72</v>
       </c>
       <c r="K33" t="s">
         <v>6</v>
@@ -1881,67 +2651,80 @@
       <c r="L33" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>0.60111000000000003</v>
-      </c>
+      <c r="M33" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C34" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="D34" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E34" t="b">
         <v>1</v>
       </c>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1">
-        <v>0.60111000000000003</v>
+      <c r="H34">
+        <v>1419.8810000000001</v>
+      </c>
+      <c r="I34" s="12">
+        <v>1.5775999999999999</v>
+      </c>
+      <c r="J34" s="14">
+        <v>0.73</v>
       </c>
       <c r="K34" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="L34" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>0.59777999999999998</v>
-      </c>
+      <c r="M34" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C35" s="2">
-        <v>4.3055555555555562E-2</v>
+        <v>4.8611111111111112E-2</v>
       </c>
       <c r="D35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35" t="b">
         <v>1</v>
       </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1">
-        <v>0.59777999999999998</v>
+      <c r="H35">
+        <v>1730.1410000000001</v>
+      </c>
+      <c r="I35" s="12">
+        <v>1.9224000000000001</v>
+      </c>
+      <c r="J35" s="14">
+        <v>0.69559000000000004</v>
       </c>
       <c r="K35" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>0.45695000000000002</v>
-      </c>
+      <c r="M35" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C36" s="2">
         <v>4.3055555555555562E-2</v>
@@ -1952,50 +2735,62 @@
       <c r="E36" t="b">
         <v>1</v>
       </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1">
-        <v>0.45695000000000002</v>
+      <c r="H36">
+        <v>1726.5519999999999</v>
+      </c>
+      <c r="I36" s="12">
+        <v>1.9184000000000001</v>
+      </c>
+      <c r="J36" s="14">
+        <v>0.60111000000000003</v>
       </c>
       <c r="K36" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>0.43382999999999999</v>
-      </c>
+      <c r="M36" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C37" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="D37" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E37" t="b">
         <v>1</v>
       </c>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1">
-        <v>0.43382999999999999</v>
+      <c r="H37">
+        <v>1706.893</v>
+      </c>
+      <c r="I37" s="12">
+        <v>1.8965000000000001</v>
+      </c>
+      <c r="J37" s="14">
+        <v>0.59667000000000003</v>
       </c>
       <c r="K37" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>0.40998000000000001</v>
-      </c>
+      <c r="M37" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C38" s="2">
         <v>4.3055555555555562E-2</v>
@@ -2006,23 +2801,29 @@
       <c r="E38" t="b">
         <v>1</v>
       </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1">
-        <v>0.40998000000000001</v>
+      <c r="H38">
+        <v>6451.2250000000004</v>
+      </c>
+      <c r="I38" s="12">
+        <v>1.9625999999999999</v>
+      </c>
+      <c r="J38" s="14">
+        <v>0.45634000000000002</v>
       </c>
       <c r="K38" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>0.1133</v>
-      </c>
+      <c r="M38" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C39" s="2">
         <v>4.3055555555555562E-2</v>
@@ -2033,23 +2834,29 @@
       <c r="E39" t="b">
         <v>1</v>
       </c>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1">
-        <v>0.1133</v>
+      <c r="H39">
+        <v>6758.4920000000002</v>
+      </c>
+      <c r="I39" s="12">
+        <v>2.0560999999999998</v>
+      </c>
+      <c r="J39" s="14">
+        <v>0.43353000000000003</v>
       </c>
       <c r="K39" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>4.2900000000000001E-2</v>
-      </c>
+      <c r="M39" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C40" s="2">
         <v>4.3055555555555562E-2</v>
@@ -2060,21 +2867,95 @@
       <c r="E40" t="b">
         <v>1</v>
       </c>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1">
-        <v>4.2900000000000001E-2</v>
+      <c r="H40">
+        <v>17432.940999999999</v>
+      </c>
+      <c r="I40" s="12">
+        <v>3.0832999999999999</v>
+      </c>
+      <c r="J40" s="14">
+        <v>0.40998000000000001</v>
       </c>
       <c r="K40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="M40" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>32117.952000000001</v>
+      </c>
+      <c r="I41" s="12">
+        <v>3.2118000000000002</v>
+      </c>
+      <c r="J41" s="14">
+        <v>0.1116</v>
+      </c>
+      <c r="K41" t="s">
+        <v>10</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M41" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>32641.157999999999</v>
+      </c>
+      <c r="I42" s="12">
+        <v>3.2641</v>
+      </c>
+      <c r="J42" s="14">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="K42" t="s">
+        <v>9</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M42" s="11" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A26:E40">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A27:E40">
-      <sortCondition descending="1" ref="A26:A40"/>
+  <autoFilter ref="A26:E42" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A27:E42">
+      <sortCondition descending="1" ref="A26:A42"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2082,22 +2963,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2111,7 +2992,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0.61973999999999996</v>
       </c>
@@ -2122,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0.52297000000000005</v>
       </c>
@@ -2133,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0.79727000000000003</v>
       </c>
@@ -2144,7 +3025,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0.60111000000000003</v>
       </c>
@@ -2155,7 +3036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0.1133</v>
       </c>
@@ -2166,7 +3047,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4.2900000000000001E-2</v>
       </c>
@@ -2177,7 +3058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0.81667000000000001</v>
       </c>
@@ -2188,7 +3069,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0.46516999999999997</v>
       </c>
@@ -2200,7 +3081,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C9">
+  <autoFilter ref="A1:C9" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C9">
       <sortCondition ref="C1:C9"/>
     </sortState>
@@ -2211,24 +3092,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -2236,7 +3117,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2247,7 +3128,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0.81667000000000001</v>
       </c>
@@ -2267,7 +3148,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0.81444000000000005</v>
       </c>
@@ -2287,7 +3168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0.81444000000000005</v>
       </c>
@@ -2307,7 +3188,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0.81222000000000005</v>
       </c>
@@ -2327,7 +3208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0.79727000000000003</v>
       </c>
@@ -2347,7 +3228,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0.73</v>
       </c>
@@ -2367,7 +3248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0.72777999999999998</v>
       </c>
@@ -2387,7 +3268,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.72777999999999998</v>
       </c>
@@ -2407,7 +3288,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>0.72333000000000003</v>
       </c>
@@ -2427,7 +3308,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>0.72111000000000003</v>
       </c>
@@ -2438,7 +3319,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>0.70667000000000002</v>
       </c>
@@ -2449,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>0.69333</v>
       </c>
@@ -2460,7 +3341,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>0.61973999999999996</v>
       </c>
@@ -2471,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>0.61602000000000001</v>
       </c>
@@ -2482,7 +3363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>0.61231000000000002</v>
       </c>
@@ -2493,7 +3374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>0.60133999999999999</v>
       </c>
@@ -2504,7 +3385,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>0.60111000000000003</v>
       </c>
@@ -2515,7 +3396,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>0.59777999999999998</v>
       </c>
@@ -2526,7 +3407,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>0.52297000000000005</v>
       </c>
@@ -2537,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>0.52175000000000005</v>
       </c>
@@ -2548,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>0.51415</v>
       </c>
@@ -2559,7 +3440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>0.50927999999999995</v>
       </c>
@@ -2570,7 +3451,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>0.46516999999999997</v>
       </c>
@@ -2581,7 +3462,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>0.45695000000000002</v>
       </c>
@@ -2592,7 +3473,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>0.43382999999999999</v>
       </c>
@@ -2603,7 +3484,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>0.40998000000000001</v>
       </c>
@@ -2614,7 +3495,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>0.1133</v>
       </c>
@@ -2625,7 +3506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>0.1105</v>
       </c>
@@ -2636,7 +3517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>0.1099</v>
       </c>
@@ -2647,7 +3528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>4.2900000000000001E-2</v>
       </c>
@@ -2658,7 +3539,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>3.4299999999999997E-2</v>
       </c>
@@ -2669,7 +3550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2.5399999999999999E-2</v>
       </c>
@@ -2681,7 +3562,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:C34">
+  <autoFilter ref="A2:C34" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C34">
       <sortCondition descending="1" ref="A2:A34"/>
     </sortState>
@@ -2691,28 +3572,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2729,7 +3610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0.81222000000000005</v>
       </c>
@@ -2746,7 +3627,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0.70667000000000002</v>
       </c>
@@ -2763,7 +3644,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0.61973999999999996</v>
       </c>
@@ -2780,7 +3661,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0.61602000000000001</v>
       </c>
@@ -2797,7 +3678,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0.61231000000000002</v>
       </c>
@@ -2814,7 +3695,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0.52297000000000005</v>
       </c>
@@ -2831,7 +3712,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0.52175000000000005</v>
       </c>
@@ -2848,7 +3729,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.1099</v>
       </c>
@@ -2865,7 +3746,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>3.4299999999999997E-2</v>
       </c>
@@ -2883,7 +3764,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E11">
+  <autoFilter ref="A2:E11" xr:uid="{00000000-0009-0000-0000-000003000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E11">
       <sortCondition descending="1" ref="A2:A11"/>
     </sortState>
@@ -2893,53 +3774,53 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0.81667000000000001</v>
       </c>
@@ -2955,14 +3836,14 @@
       <c r="E3">
         <v>40</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0.81444000000000005</v>
       </c>
@@ -2978,14 +3859,14 @@
       <c r="E4">
         <v>40</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0.81444000000000005</v>
       </c>
@@ -3001,14 +3882,14 @@
       <c r="E5">
         <v>40</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0.60133999999999999</v>
       </c>
@@ -3024,14 +3905,14 @@
       <c r="E6">
         <v>40</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0.51415</v>
       </c>
@@ -3047,14 +3928,14 @@
       <c r="E7">
         <v>40</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0.50927999999999995</v>
       </c>
@@ -3070,14 +3951,14 @@
       <c r="E8">
         <v>40</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0.46516999999999997</v>
       </c>
@@ -3087,20 +3968,20 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E9">
         <v>40</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>1</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.1105</v>
       </c>
@@ -3116,14 +3997,14 @@
       <c r="E10">
         <v>40</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2.5399999999999999E-2</v>
       </c>
@@ -3139,37 +4020,37 @@
       <c r="E11">
         <v>40</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G11"/>
+  <autoFilter ref="A2:G11" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -3178,7 +4059,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3201,7 +4082,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0.79727000000000003</v>
       </c>
@@ -3211,14 +4092,14 @@
       <c r="C3" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="5" t="b">
+      <c r="E3" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0.73</v>
       </c>
@@ -3228,14 +4109,14 @@
       <c r="C4" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5" t="b">
+      <c r="E4" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0.72777999999999998</v>
       </c>
@@ -3245,14 +4126,14 @@
       <c r="C5" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="5" t="b">
+      <c r="E5" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0.72777999999999998</v>
       </c>
@@ -3262,14 +4143,14 @@
       <c r="C6" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0.72333000000000003</v>
       </c>
@@ -3279,14 +4160,14 @@
       <c r="C7" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0.72111000000000003</v>
       </c>
@@ -3296,14 +4177,14 @@
       <c r="C8" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="5" t="b">
+      <c r="E8" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0.69333</v>
       </c>
@@ -3313,14 +4194,14 @@
       <c r="C9" s="2">
         <v>4.8611111111111112E-2</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="5" t="b">
+      <c r="E9" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.60111000000000003</v>
       </c>
@@ -3330,14 +4211,14 @@
       <c r="C10" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="5" t="b">
+      <c r="E10" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>0.59777999999999998</v>
       </c>
@@ -3347,14 +4228,14 @@
       <c r="C11" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="5" t="b">
+      <c r="E11" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>0.45695000000000002</v>
       </c>
@@ -3364,14 +4245,14 @@
       <c r="C12" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="5" t="b">
+      <c r="E12" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>0.43382999999999999</v>
       </c>
@@ -3381,15 +4262,14 @@
       <c r="C13" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="5" t="b">
+      <c r="E13" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>0.40998000000000001</v>
       </c>
@@ -3399,14 +4279,14 @@
       <c r="C14" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="5" t="b">
+      <c r="E14" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>0.1133</v>
       </c>
@@ -3416,14 +4296,14 @@
       <c r="C15" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="5" t="b">
+      <c r="E15" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>4.2900000000000001E-2</v>
       </c>
@@ -3433,89 +4313,89 @@
       <c r="C16" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="5" t="b">
+      <c r="E16" s="4" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E16"/>
+  <autoFilter ref="A2:E16" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A11">
+  <autoFilter ref="A1:A11" xr:uid="{00000000-0009-0000-0000-000006000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A11">
       <sortCondition ref="A1:A11"/>
     </sortState>

</xml_diff>

<commit_message>
Added bit penalty to % correctness row
Under the "Compare All" tab, I made it easier to select the best results by filtering the lowest to highest bit penalty per % correctness. Some data was VERY close with slight trade-offs. Note, some of the "best" is fractionally better than the next result.
</commit_message>
<xml_diff>
--- a/stats_workbook.xlsx
+++ b/stats_workbook.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\westw\Documents\8_2023_Spring\EENG311_Information Systems Science 2\ISSII_Group3Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774032AD-1D51-4F9B-BBD3-1D8354E753FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24929146-EE08-4286-B3EE-1B89470D85B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Stats" sheetId="1" r:id="rId1"/>
     <sheet name="LSTM Multi" sheetId="9" r:id="rId2"/>
     <sheet name="NN_NoLSTM" sheetId="10" r:id="rId3"/>
     <sheet name="NAR_NN" sheetId="11" r:id="rId4"/>
-    <sheet name="Best of" sheetId="6" r:id="rId5"/>
-    <sheet name="All Stats" sheetId="5" r:id="rId6"/>
+    <sheet name="Compare All" sheetId="12" r:id="rId5"/>
+    <sheet name="Best of" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
     <sheet name="seq" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'All Stats'!$A$2:$C$34</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Best of'!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Best of'!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Compare All'!$A$2:$G$67</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'LSTM Multi'!$B$2:$K$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">NAR_NN!$B$2:$K$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NN_NoLSTM!$B$2:$M$9</definedName>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="114">
   <si>
     <t>LSTM_Multichannel</t>
   </si>
@@ -153,13 +153,7 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>All stats</t>
-  </si>
-  <si>
     <t>Method</t>
-  </si>
-  <si>
-    <t>Best of</t>
   </si>
   <si>
     <t>Data Sets</t>
@@ -1253,6 +1247,46 @@
 0 probabilities forecasted between 70% and 80%.
 0 probabilities forecasted between 80% and 90%.
 0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>ALL STATS</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart1_test.mat.
+Total penalty: 1532.616 bits (1.7029 bits per symbol).
+Correctly predicted 60.000% of symbols.
+5404 probabilities forecasted between 0% and 1%; actual occurrence rate 0.52%.
+339 probabilities forecasted between 1% and 5%; actual occurrence rate 9.14%.
+550 probabilities forecasted between 5% and 10%; actual occurrence rate 16.55%.
+560 probabilities forecasted between 10% and 20%; actual occurrence rate 18.75%.
+201 probabilities forecasted between 20% and 30%; actual occurrence rate 22.39%.
+34 probabilities forecasted between 30% and 40%; actual occurrence rate 26.47%.
+113 probabilities forecasted between 40% and 50%; actual occurrence rate 45.13%.
+113 probabilities forecasted between 50% and 60%; actual occurrence rate 43.36%.
+61 probabilities forecasted between 60% and 70%; actual occurrence rate 60.66%.
+724 probabilities forecasted between 70% and 80%; actual occurrence rate 62.71%.
+1 probabilities forecasted between 80% and 90%; actual occurrence rate 0.00%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>Symbol Machine processed 900 out of 900 symbols in sequence_heart1_test.mat.
+Total penalty: 1667.097 bits (1.8523 bits per symbol).
+Correctly predicted 62.444% of symbols.
+2437 probabilities forecasted between 0% and 1%; actual occurrence rate 0.37%.
+1441 probabilities forecasted between 1% and 5%; actual occurrence rate 0.21%.
+1225 probabilities forecasted between 5% and 10%; actual occurrence rate 0.73%.
+392 probabilities forecasted between 10% and 20%; actual occurrence rate 2.04%.
+1645 probabilities forecasted between 20% and 30%; actual occurrence rate 17.99%.
+948 probabilities forecasted between 30% and 40%; actual occurrence rate 60.02%.
+8 probabilities forecasted between 40% and 50%; actual occurrence rate 75.00%.
+1 probabilities forecasted between 50% and 60%; actual occurrence rate 0.00%.
+2 probabilities forecasted between 60% and 70%; actual occurrence rate 0.00%.
+0 probabilities forecasted between 70% and 80%.
+1 probabilities forecasted between 80% and 90%; actual occurrence rate 0.00%.
+0 probabilities forecasted between 90% and 100%.</t>
+  </si>
+  <si>
+    <t>bit penalty per % correctness</t>
   </si>
 </sst>
 </file>
@@ -2202,10 +2236,10 @@
         <v>5</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>1</v>
@@ -2214,10 +2248,10 @@
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2250,7 +2284,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2283,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2316,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2349,7 +2383,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2382,7 +2416,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2415,7 +2449,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2448,7 +2482,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2481,7 +2515,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2514,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2551,10 +2585,10 @@
         <v>30</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J14" s="14" t="s">
         <v>1</v>
@@ -2563,7 +2597,7 @@
         <v>2</v>
       </c>
       <c r="L14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2602,7 +2636,7 @@
         <v>11</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2641,7 +2675,7 @@
         <v>11</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2680,7 +2714,7 @@
         <v>11</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2719,7 +2753,7 @@
         <v>11</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2758,7 +2792,7 @@
         <v>11</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2797,7 +2831,7 @@
         <v>11</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2831,7 +2865,7 @@
         <v>11</v>
       </c>
       <c r="M21" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2870,7 +2904,7 @@
         <v>11</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2909,7 +2943,7 @@
         <v>11</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2941,10 +2975,10 @@
         <v>19</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J26" s="14" t="s">
         <v>1</v>
@@ -2953,7 +2987,7 @@
         <v>2</v>
       </c>
       <c r="L26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2986,7 +3020,7 @@
         <v>16</v>
       </c>
       <c r="M27" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3019,7 +3053,7 @@
         <v>16</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3052,7 +3086,7 @@
         <v>16</v>
       </c>
       <c r="M29" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3085,7 +3119,7 @@
         <v>16</v>
       </c>
       <c r="M30" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3118,13 +3152,13 @@
         <v>16</v>
       </c>
       <c r="M31" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C32" s="2">
         <v>4.3055555555555562E-2</v>
@@ -3151,7 +3185,7 @@
         <v>16</v>
       </c>
       <c r="M32" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3184,7 +3218,7 @@
         <v>16</v>
       </c>
       <c r="M33" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3217,7 +3251,7 @@
         <v>16</v>
       </c>
       <c r="M34" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3250,7 +3284,7 @@
         <v>16</v>
       </c>
       <c r="M35" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3283,7 +3317,7 @@
         <v>16</v>
       </c>
       <c r="M36" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3316,7 +3350,7 @@
         <v>16</v>
       </c>
       <c r="M37" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3349,7 +3383,7 @@
         <v>16</v>
       </c>
       <c r="M38" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3382,7 +3416,7 @@
         <v>16</v>
       </c>
       <c r="M39" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3415,7 +3449,7 @@
         <v>16</v>
       </c>
       <c r="M40" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3448,7 +3482,7 @@
         <v>16</v>
       </c>
       <c r="M41" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3481,7 +3515,7 @@
         <v>16</v>
       </c>
       <c r="M42" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3498,8 +3532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9967961-8901-4860-80ED-288F2B5CB12C}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3541,10 +3575,10 @@
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>1</v>
@@ -3553,10 +3587,10 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3589,7 +3623,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3622,7 +3656,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3655,7 +3689,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3688,7 +3722,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3721,7 +3755,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3754,7 +3788,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3787,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3820,7 +3854,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3853,7 +3887,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3885,7 +3919,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3918,7 +3952,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3951,7 +3985,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3984,7 +4018,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4017,7 +4051,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4050,7 +4084,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4083,7 +4117,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4116,7 +4150,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4149,7 +4183,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4182,7 +4216,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4215,7 +4249,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4248,7 +4282,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4281,7 +4315,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4314,7 +4348,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4347,7 +4381,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4380,7 +4414,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4413,7 +4447,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4446,7 +4480,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4479,7 +4513,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4512,7 +4546,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4619,7 +4653,7 @@
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4669,10 +4703,10 @@
         <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>1</v>
@@ -4681,7 +4715,7 @@
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4720,7 +4754,7 @@
         <v>11</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4759,7 +4793,7 @@
         <v>11</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4798,7 +4832,7 @@
         <v>11</v>
       </c>
       <c r="M5" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4837,7 +4871,7 @@
         <v>11</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4846,7 +4880,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D7">
         <v>250</v>
@@ -4876,7 +4910,7 @@
         <v>11</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4915,7 +4949,7 @@
         <v>11</v>
       </c>
       <c r="M8" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4954,7 +4988,7 @@
         <v>11</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4963,7 +4997,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D10">
         <v>250</v>
@@ -4993,7 +5027,7 @@
         <v>11</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5002,7 +5036,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D11">
         <v>250</v>
@@ -5032,7 +5066,7 @@
         <v>11</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5071,7 +5105,7 @@
         <v>11</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5110,7 +5144,7 @@
         <v>11</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5149,7 +5183,7 @@
         <v>11</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5188,7 +5222,7 @@
         <v>11</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5227,7 +5261,7 @@
         <v>11</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5236,7 +5270,7 @@
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D17">
         <v>250</v>
@@ -5266,7 +5300,7 @@
         <v>11</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5275,7 +5309,7 @@
         <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D18">
         <v>250</v>
@@ -5305,7 +5339,7 @@
         <v>11</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5344,7 +5378,7 @@
         <v>11</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5383,7 +5417,7 @@
         <v>11</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5464,10 +5498,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1108626-858A-4027-BC1B-7377445CA427}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F19" sqref="F19:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5510,10 +5544,10 @@
         <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>1</v>
@@ -5522,13 +5556,13 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2">
         <v>4.3055555555555562E-2</v>
@@ -5540,94 +5574,94 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>6758.4920000000002</v>
+        <v>951.06399999999996</v>
       </c>
       <c r="G3" s="11">
-        <v>2.0560999999999998</v>
+        <v>0.999</v>
       </c>
       <c r="H3" s="13">
-        <v>0.43353000000000003</v>
+        <v>0.79096999999999995</v>
       </c>
       <c r="I3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
       </c>
       <c r="F4">
-        <v>6451.2250000000004</v>
+        <v>1682.8320000000001</v>
       </c>
       <c r="G4" s="11">
-        <v>1.9625999999999999</v>
+        <v>1.8697999999999999</v>
       </c>
       <c r="H4" s="13">
-        <v>0.45634000000000002</v>
+        <v>0.73</v>
       </c>
       <c r="I4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>17432.940999999999</v>
+        <v>1419.8810000000001</v>
       </c>
       <c r="G5" s="11">
-        <v>3.0832999999999999</v>
+        <v>1.5775999999999999</v>
       </c>
       <c r="H5" s="13">
-        <v>0.40998000000000001</v>
+        <v>0.73</v>
       </c>
       <c r="I5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C6" s="2">
         <v>4.3055555555555562E-2</v>
@@ -5654,13 +5688,13 @@
         <v>16</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
         <v>4.3055555555555562E-2</v>
@@ -5672,55 +5706,55 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>1726.5519999999999</v>
+        <v>1353.373</v>
       </c>
       <c r="G7" s="11">
-        <v>1.9184000000000001</v>
+        <v>1.5037</v>
       </c>
       <c r="H7" s="13">
-        <v>0.60111000000000003</v>
+        <v>0.72889000000000004</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>1706.893</v>
+        <v>1541.8119999999999</v>
       </c>
       <c r="G8" s="11">
-        <v>1.8965000000000001</v>
+        <v>1.7131000000000001</v>
       </c>
       <c r="H8" s="13">
-        <v>0.59667000000000003</v>
+        <v>0.72777999999999998</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5734,17 +5768,17 @@
       <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="b">
-        <v>1</v>
+      <c r="E9" t="s">
+        <v>28</v>
       </c>
       <c r="F9">
-        <v>1353.373</v>
+        <v>1668.934</v>
       </c>
       <c r="G9" s="11">
-        <v>1.5037</v>
+        <v>1.8544</v>
       </c>
       <c r="H9" s="13">
-        <v>0.72889000000000004</v>
+        <v>0.72221999999999997</v>
       </c>
       <c r="I9" t="s">
         <v>6</v>
@@ -5753,7 +5787,7 @@
         <v>16</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5767,17 +5801,17 @@
       <c r="D10" t="s">
         <v>24</v>
       </c>
-      <c r="E10" t="b">
-        <v>1</v>
+      <c r="E10" t="s">
+        <v>27</v>
       </c>
       <c r="F10">
-        <v>1541.8119999999999</v>
+        <v>1097.5930000000001</v>
       </c>
       <c r="G10" s="11">
-        <v>1.7131000000000001</v>
+        <v>1.2195</v>
       </c>
       <c r="H10" s="13">
-        <v>0.72777999999999998</v>
+        <v>0.72</v>
       </c>
       <c r="I10" t="s">
         <v>6</v>
@@ -5795,22 +5829,22 @@
         <v>6</v>
       </c>
       <c r="C11" s="2">
-        <v>4.3055555555555562E-2</v>
+        <v>4.8611111111111112E-2</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>1682.8320000000001</v>
+        <v>1730.1410000000001</v>
       </c>
       <c r="G11" s="11">
-        <v>1.8697999999999999</v>
+        <v>1.9224000000000001</v>
       </c>
       <c r="H11" s="13">
-        <v>0.73</v>
+        <v>0.69559000000000004</v>
       </c>
       <c r="I11" t="s">
         <v>6</v>
@@ -5819,13 +5853,13 @@
         <v>16</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2">
         <v>4.3055555555555562E-2</v>
@@ -5833,101 +5867,101 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
-        <v>28</v>
+      <c r="E12" t="b">
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>1668.934</v>
+        <v>1726.5519999999999</v>
       </c>
       <c r="G12" s="11">
-        <v>1.8544</v>
+        <v>1.9184000000000001</v>
       </c>
       <c r="H12" s="13">
-        <v>0.72221999999999997</v>
+        <v>0.60111000000000003</v>
       </c>
       <c r="I12" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>1097.5930000000001</v>
+        <v>1706.893</v>
       </c>
       <c r="G13" s="11">
-        <v>1.2195</v>
+        <v>1.8965000000000001</v>
       </c>
       <c r="H13" s="13">
-        <v>0.72</v>
+        <v>0.59667000000000003</v>
       </c>
       <c r="I13" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2">
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
       </c>
       <c r="F14">
-        <v>1419.8810000000001</v>
+        <v>6451.2250000000004</v>
       </c>
       <c r="G14" s="11">
-        <v>1.5775999999999999</v>
+        <v>1.9625999999999999</v>
       </c>
       <c r="H14" s="13">
-        <v>0.73</v>
+        <v>0.45634000000000002</v>
       </c>
       <c r="I14" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2">
-        <v>4.8611111111111112E-2</v>
+        <v>4.3055555555555562E-2</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
@@ -5936,28 +5970,28 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>1730.1410000000001</v>
+        <v>6758.4920000000002</v>
       </c>
       <c r="G15" s="11">
-        <v>1.9224000000000001</v>
+        <v>2.0560999999999998</v>
       </c>
       <c r="H15" s="13">
-        <v>0.69559000000000004</v>
+        <v>0.43353000000000003</v>
       </c>
       <c r="I15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2">
         <v>4.3055555555555562E-2</v>
@@ -5969,28 +6003,28 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>32641.157999999999</v>
+        <v>17432.940999999999</v>
       </c>
       <c r="G16" s="11">
-        <v>3.2641</v>
+        <v>3.0832999999999999</v>
       </c>
       <c r="H16" s="13">
-        <v>3.0300000000000001E-2</v>
+        <v>0.40998000000000001</v>
       </c>
       <c r="I16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2">
         <v>4.3055555555555562E-2</v>
@@ -6002,28 +6036,28 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>951.06399999999996</v>
+        <v>32117.952000000001</v>
       </c>
       <c r="G17" s="11">
-        <v>0.999</v>
+        <v>3.2118000000000002</v>
       </c>
       <c r="H17" s="13">
-        <v>0.79096999999999995</v>
+        <v>0.1116</v>
       </c>
       <c r="I17" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="2">
         <v>4.3055555555555562E-2</v>
@@ -6035,31 +6069,1894 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>32117.952000000001</v>
+        <v>32641.157999999999</v>
       </c>
       <c r="G18" s="11">
-        <v>3.2118000000000002</v>
+        <v>3.2641</v>
       </c>
       <c r="H18" s="13">
-        <v>0.1116</v>
+        <v>3.0300000000000001E-2</v>
       </c>
       <c r="I18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K18" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19">
+        <v>1532.616</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1.7029000000000001</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I19" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20">
+        <v>1667.097</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1.8523000000000001</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.62444</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <autoFilter ref="B2:K18" xr:uid="{E1108626-858A-4027-BC1B-7377445CA427}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:K18">
+      <sortCondition descending="1" ref="H2:H18"/>
+    </sortState>
+  </autoFilter>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C92FFF-D1FD-47B8-800D-712537A126E1}">
+  <dimension ref="A1:O79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="89.140625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>B3/D3</f>
+        <v>831.08243694145654</v>
+      </c>
+      <c r="B3">
+        <v>712.35400000000004</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0.74829999999999997</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0.85714000000000001</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3">
+        <v>712.35400000000004</v>
+      </c>
+      <c r="K3" s="11">
+        <v>0.74829999999999997</v>
+      </c>
+      <c r="L3" s="13">
+        <v>0.85714000000000001</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>B4/D4</f>
+        <v>831.08593695312311</v>
+      </c>
+      <c r="B4">
+        <v>712.35699999999997</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.74829999999999997</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0.85714000000000001</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="J4">
+        <v>824.94299999999998</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0.91659999999999997</v>
+      </c>
+      <c r="L4" s="13">
+        <v>0.81444000000000005</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>B5/D5</f>
+        <v>984.79482297421998</v>
+      </c>
+      <c r="B5">
+        <v>843.07299999999998</v>
+      </c>
+      <c r="C5">
+        <v>0.88560000000000005</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.85609000000000002</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5">
+        <v>1141.374</v>
+      </c>
+      <c r="K5">
+        <v>1.2682</v>
+      </c>
+      <c r="L5" s="13">
+        <v>0.75667000000000006</v>
+      </c>
+      <c r="M5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>B6/D6</f>
+        <v>1012.8959776042433</v>
+      </c>
+      <c r="B6">
+        <v>824.94299999999998</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0.91659999999999997</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.81444000000000005</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6">
+        <v>9691.6569999999992</v>
+      </c>
+      <c r="K6">
+        <v>1.7141</v>
+      </c>
+      <c r="L6" s="13">
+        <v>0.62133000000000005</v>
+      </c>
+      <c r="M6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>B7/D7</f>
+        <v>1012.8419527528117</v>
+      </c>
+      <c r="B7">
+        <v>824.899</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.91659999999999997</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.81444000000000005</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7">
+        <v>5401.1049999999996</v>
+      </c>
+      <c r="K7">
+        <v>1.6432</v>
+      </c>
+      <c r="L7" s="13">
+        <v>0.52997000000000005</v>
+      </c>
+      <c r="M7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>B8/D8</f>
+        <v>1013.5281080485386</v>
+      </c>
+      <c r="B8">
+        <v>827.71799999999996</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.91969999999999996</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.81667000000000001</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8">
+        <v>6210.174</v>
+      </c>
+      <c r="K8" s="11">
+        <v>1.8893</v>
+      </c>
+      <c r="L8" s="13">
+        <v>0.46425</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>B9/D9</f>
+        <v>1013.9358614862797</v>
+      </c>
+      <c r="B9">
+        <v>828.05100000000004</v>
+      </c>
+      <c r="C9">
+        <v>0.92010000000000003</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.81667000000000001</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9">
+        <v>31763.324000000001</v>
+      </c>
+      <c r="K9" s="11">
+        <v>3.1762999999999999</v>
+      </c>
+      <c r="L9" s="13">
+        <v>0.11459999999999999</v>
+      </c>
+      <c r="M9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>B10/D10</f>
+        <v>1123.7383300460224</v>
+      </c>
+      <c r="B10">
+        <v>854.60299999999995</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.89770000000000005</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0.76049999999999995</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="J10">
+        <v>38303.574000000001</v>
+      </c>
+      <c r="K10">
+        <v>3.8304</v>
+      </c>
+      <c r="L10" s="13">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>B11/D11</f>
+        <v>1202.402113860197</v>
+      </c>
+      <c r="B11">
+        <v>951.06399999999996</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0.999</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0.79096999999999995</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>B12/D12</f>
+        <v>1202.4883843464099</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1004.174</v>
+      </c>
+      <c r="C12">
+        <v>1.0548</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0.83508000000000004</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>B13/D13</f>
+        <v>1184.6130266320076</v>
+      </c>
+      <c r="B13" s="20">
+        <v>966.12300000000005</v>
+      </c>
+      <c r="C13">
+        <v>1.0734999999999999</v>
+      </c>
+      <c r="D13" s="13">
+        <v>0.81555999999999995</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>B14/D14</f>
+        <v>1266.6079157824056</v>
+      </c>
+      <c r="B14">
+        <v>1056.3889999999999</v>
+      </c>
+      <c r="C14">
+        <v>1.1096999999999999</v>
+      </c>
+      <c r="D14" s="13">
+        <v>0.83403000000000005</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>B15/D15</f>
+        <v>1499.750748980895</v>
+      </c>
+      <c r="B15">
+        <v>1221.4570000000001</v>
+      </c>
+      <c r="C15">
+        <v>1.3572</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0.81444000000000005</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>B16/D16</f>
+        <v>1508.4171435368125</v>
+      </c>
+      <c r="B16">
+        <v>1141.374</v>
+      </c>
+      <c r="C16">
+        <v>1.2682</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0.75667000000000006</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>B17/D17</f>
+        <v>1515.8403320072687</v>
+      </c>
+      <c r="B17">
+        <v>1234.5609999999999</v>
+      </c>
+      <c r="C17" s="11">
+        <v>1.3716999999999999</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0.81444000000000005</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>B18/D18</f>
+        <v>1524.4347222222225</v>
+      </c>
+      <c r="B18">
+        <v>1097.5930000000001</v>
+      </c>
+      <c r="C18" s="11">
+        <v>1.2195</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.72</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>B19/D19</f>
+        <v>1629.6629156270687</v>
+      </c>
+      <c r="B19" s="20">
+        <v>1280.1980000000001</v>
+      </c>
+      <c r="C19">
+        <v>1.4224000000000001</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.78556000000000004</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f>B20/D20</f>
+        <v>1631.2310499526677</v>
+      </c>
+      <c r="B20">
+        <v>1188.9880000000001</v>
+      </c>
+      <c r="C20" s="11">
+        <v>1.3210999999999999</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0.72889000000000004</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>B21/D21</f>
+        <v>1789.2273392512755</v>
+      </c>
+      <c r="B21">
+        <v>1308.1220000000001</v>
+      </c>
+      <c r="C21">
+        <v>1.4535</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.73111000000000004</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>B22/D22</f>
+        <v>1856.7589073797144</v>
+      </c>
+      <c r="B22">
+        <v>1353.373</v>
+      </c>
+      <c r="C22" s="11">
+        <v>1.5037</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0.72889000000000004</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>B23/D23</f>
+        <v>1916.2186739415333</v>
+      </c>
+      <c r="B23">
+        <v>1432.91</v>
+      </c>
+      <c r="C23">
+        <v>1.5921000000000001</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.74778000000000011</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>B24/D24</f>
+        <v>1945.0424657534247</v>
+      </c>
+      <c r="B24">
+        <v>1419.8810000000001</v>
+      </c>
+      <c r="C24" s="11">
+        <v>1.5775999999999999</v>
+      </c>
+      <c r="D24" s="13">
+        <v>0.73</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>B25/D25</f>
+        <v>2118.5138365989719</v>
+      </c>
+      <c r="B25">
+        <v>1541.8119999999999</v>
+      </c>
+      <c r="C25" s="11">
+        <v>1.7131000000000001</v>
+      </c>
+      <c r="D25" s="13">
+        <v>0.72777999999999998</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f>B26/D26</f>
+        <v>2305.2493150684932</v>
+      </c>
+      <c r="B26">
+        <v>1682.8320000000001</v>
+      </c>
+      <c r="C26" s="11">
+        <v>1.8697999999999999</v>
+      </c>
+      <c r="D26" s="13">
+        <v>0.73</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f>B27/D27</f>
+        <v>2310.8388025809309</v>
+      </c>
+      <c r="B27">
+        <v>1668.934</v>
+      </c>
+      <c r="C27" s="11">
+        <v>1.8544</v>
+      </c>
+      <c r="D27" s="13">
+        <v>0.72221999999999997</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f>B28/D28</f>
+        <v>15598.244089292322</v>
+      </c>
+      <c r="B28">
+        <v>9691.6569999999992</v>
+      </c>
+      <c r="C28">
+        <v>1.7141</v>
+      </c>
+      <c r="D28" s="13">
+        <v>0.62133000000000005</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f>B29/D29</f>
+        <v>2487.2999899366005</v>
+      </c>
+      <c r="B29">
+        <v>1730.1410000000001</v>
+      </c>
+      <c r="C29" s="11">
+        <v>1.9224000000000001</v>
+      </c>
+      <c r="D29" s="13">
+        <v>0.69559000000000004</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f>B30/D30</f>
+        <v>15627.754446840594</v>
+      </c>
+      <c r="B30">
+        <v>9638.1049999999996</v>
+      </c>
+      <c r="C30" s="11">
+        <v>1.7074</v>
+      </c>
+      <c r="D30" s="13">
+        <v>0.61673</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>B31/D31</f>
+        <v>15697.70169084087</v>
+      </c>
+      <c r="B31">
+        <v>9664.6039999999994</v>
+      </c>
+      <c r="C31" s="11">
+        <v>1.7093</v>
+      </c>
+      <c r="D31" s="13">
+        <v>0.61567000000000005</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f>B32/D32</f>
+        <v>2554.36</v>
+      </c>
+      <c r="B32">
+        <v>1532.616</v>
+      </c>
+      <c r="C32" s="11">
+        <v>1.7029000000000001</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f>B33/D33</f>
+        <v>16109.686470261981</v>
+      </c>
+      <c r="B33" s="3">
+        <v>9875.56</v>
+      </c>
+      <c r="C33">
+        <v>1.7466999999999999</v>
+      </c>
+      <c r="D33" s="13">
+        <v>0.61302000000000001</v>
+      </c>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f>B34/D34</f>
+        <v>16186.907144367973</v>
+      </c>
+      <c r="B34">
+        <v>9948.6350000000002</v>
+      </c>
+      <c r="C34">
+        <v>1.7596000000000001</v>
+      </c>
+      <c r="D34" s="13">
+        <v>0.61460999999999999</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f>B35/D35</f>
+        <v>17067.332956397382</v>
+      </c>
+      <c r="B35">
+        <v>10263.27</v>
+      </c>
+      <c r="C35">
+        <v>1.7625999999999999</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.60133999999999999</v>
+      </c>
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>B36/D36</f>
+        <v>16606.144611811655</v>
+      </c>
+      <c r="B36">
+        <v>10153.495000000001</v>
+      </c>
+      <c r="C36" s="11">
+        <v>1.7958000000000001</v>
+      </c>
+      <c r="D36" s="13">
+        <v>0.61143000000000003</v>
+      </c>
+      <c r="E36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>B37/D37</f>
+        <v>2669.7472935750434</v>
+      </c>
+      <c r="B37">
+        <v>1667.097</v>
+      </c>
+      <c r="C37" s="11">
+        <v>1.8523000000000001</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.62444</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f>B38/D38</f>
+        <v>16785.528985266239</v>
+      </c>
+      <c r="B38" s="20">
+        <v>10093.81</v>
+      </c>
+      <c r="C38" s="22">
+        <v>1.7853000000000001</v>
+      </c>
+      <c r="D38" s="23">
+        <v>0.60133999999999999</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>B39/D39</f>
+        <v>16908.685602155187</v>
+      </c>
+      <c r="B39">
+        <v>10167.869000000001</v>
+      </c>
+      <c r="C39">
+        <v>1.7983</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.60133999999999999</v>
+      </c>
+      <c r="E39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f>B40/D40</f>
+        <v>17067.332956397382</v>
+      </c>
+      <c r="B40">
+        <v>10263.27</v>
+      </c>
+      <c r="C40">
+        <v>1.8151999999999999</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.60133999999999999</v>
+      </c>
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f>B41/D41</f>
+        <v>10191.341019302978</v>
+      </c>
+      <c r="B41">
+        <v>5401.1049999999996</v>
+      </c>
+      <c r="C41">
+        <v>1.6432</v>
+      </c>
+      <c r="D41" s="13">
+        <v>0.52997000000000005</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>77</v>
       </c>
     </row>
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f>B42/D42</f>
+        <v>10442.956574946937</v>
+      </c>
+      <c r="B42">
+        <v>5461.3530000000001</v>
+      </c>
+      <c r="C42" s="11">
+        <v>1.6615</v>
+      </c>
+      <c r="D42" s="13">
+        <v>0.52297000000000005</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f>B43/D43</f>
+        <v>2860.6985435835554</v>
+      </c>
+      <c r="B43">
+        <v>1706.893</v>
+      </c>
+      <c r="C43" s="11">
+        <v>1.8965000000000001</v>
+      </c>
+      <c r="D43" s="13">
+        <v>0.59667000000000003</v>
+      </c>
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f>B44/D44</f>
+        <v>2872.2729616875445</v>
+      </c>
+      <c r="B44">
+        <v>1726.5519999999999</v>
+      </c>
+      <c r="C44" s="11">
+        <v>1.9184000000000001</v>
+      </c>
+      <c r="D44" s="13">
+        <v>0.60111000000000003</v>
+      </c>
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f>B45/D45</f>
+        <v>10557.152417920721</v>
+      </c>
+      <c r="B45">
+        <v>5521.0739999999996</v>
+      </c>
+      <c r="C45" s="11">
+        <v>1.6797</v>
+      </c>
+      <c r="D45" s="13">
+        <v>0.52297000000000005</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f>B46/D46</f>
+        <v>10564.965979875418</v>
+      </c>
+      <c r="B46">
+        <v>5512.2709999999997</v>
+      </c>
+      <c r="C46">
+        <v>1.677</v>
+      </c>
+      <c r="D46" s="13">
+        <v>0.52175000000000005</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f>B47/D47</f>
+        <v>2951.0559048084538</v>
+      </c>
+      <c r="B47">
+        <v>1750.95</v>
+      </c>
+      <c r="C47" s="11">
+        <v>1.9455</v>
+      </c>
+      <c r="D47" s="13">
+        <v>0.59333000000000002</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f>B48/D48</f>
+        <v>11031.856738925542</v>
+      </c>
+      <c r="B48">
+        <v>5618.3040000000001</v>
+      </c>
+      <c r="C48" s="11">
+        <v>1.7092000000000001</v>
+      </c>
+      <c r="D48" s="13">
+        <v>0.50927999999999995</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f>B49/D49</f>
+        <v>11071.055215205781</v>
+      </c>
+      <c r="B49">
+        <v>5638.2669999999998</v>
+      </c>
+      <c r="C49" s="11">
+        <v>1.7153</v>
+      </c>
+      <c r="D49" s="13">
+        <v>0.50927999999999995</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f>B50/D50</f>
+        <v>13376.788368336025</v>
+      </c>
+      <c r="B50">
+        <v>6210.174</v>
+      </c>
+      <c r="C50" s="11">
+        <v>1.8893</v>
+      </c>
+      <c r="D50" s="13">
+        <v>0.46425</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f>B51/D51</f>
+        <v>13475.700974894315</v>
+      </c>
+      <c r="B51">
+        <v>6247.8739999999998</v>
+      </c>
+      <c r="C51" s="11">
+        <v>1.9008</v>
+      </c>
+      <c r="D51" s="13">
+        <v>0.46364</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f>B52/D52</f>
+        <v>13523.403438419862</v>
+      </c>
+      <c r="B52" s="20">
+        <v>6340.0420000000004</v>
+      </c>
+      <c r="C52" s="22">
+        <v>1.9288000000000001</v>
+      </c>
+      <c r="D52" s="23">
+        <v>0.46882000000000001</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f>B53/D53</f>
+        <v>14136.882587544374</v>
+      </c>
+      <c r="B53">
+        <v>6451.2250000000004</v>
+      </c>
+      <c r="C53" s="11">
+        <v>1.9625999999999999</v>
+      </c>
+      <c r="D53" s="13">
+        <v>0.45634000000000002</v>
+      </c>
+      <c r="E53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f>B54/D54</f>
+        <v>15589.444790441261</v>
+      </c>
+      <c r="B54">
+        <v>6758.4920000000002</v>
+      </c>
+      <c r="C54" s="11">
+        <v>2.0560999999999998</v>
+      </c>
+      <c r="D54" s="13">
+        <v>0.43353000000000003</v>
+      </c>
+      <c r="E54" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f>B55/D55</f>
+        <v>42521.442509390698</v>
+      </c>
+      <c r="B55">
+        <v>17432.940999999999</v>
+      </c>
+      <c r="C55" s="11">
+        <v>3.0832999999999999</v>
+      </c>
+      <c r="D55" s="13">
+        <v>0.40998000000000001</v>
+      </c>
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f>B56/D56</f>
+        <v>277166.87609075045</v>
+      </c>
+      <c r="B56">
+        <v>31763.324000000001</v>
+      </c>
+      <c r="C56" s="11">
+        <v>3.1762999999999999</v>
+      </c>
+      <c r="D56" s="13">
+        <v>0.11459999999999999</v>
+      </c>
+      <c r="E56" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f>B57/D57</f>
+        <v>280624.26431718061</v>
+      </c>
+      <c r="B57">
+        <v>31850.853999999999</v>
+      </c>
+      <c r="C57">
+        <v>3.1850999999999998</v>
+      </c>
+      <c r="D57" s="13">
+        <v>0.11349999999999999</v>
+      </c>
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f>B58/D58</f>
+        <v>283078.10810810811</v>
+      </c>
+      <c r="B58">
+        <v>32469.059000000001</v>
+      </c>
+      <c r="C58">
+        <v>3.2469000000000001</v>
+      </c>
+      <c r="D58" s="13">
+        <v>0.1147</v>
+      </c>
+      <c r="E58" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f>B59/D59</f>
+        <v>283109.48200175591</v>
+      </c>
+      <c r="B59">
+        <v>32246.17</v>
+      </c>
+      <c r="C59" s="11">
+        <v>3.2246000000000001</v>
+      </c>
+      <c r="D59" s="13">
+        <v>0.1139</v>
+      </c>
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f>B60/D60</f>
+        <v>287795.26881720428</v>
+      </c>
+      <c r="B60">
+        <v>32117.952000000001</v>
+      </c>
+      <c r="C60" s="11">
+        <v>3.2118000000000002</v>
+      </c>
+      <c r="D60" s="13">
+        <v>0.1116</v>
+      </c>
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f>B61/D61</f>
+        <v>292607.75342465757</v>
+      </c>
+      <c r="B61">
+        <v>32040.548999999999</v>
+      </c>
+      <c r="C61">
+        <v>3.2040999999999999</v>
+      </c>
+      <c r="D61" s="13">
+        <v>0.10949999999999999</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f>B62/D62</f>
+        <v>977131.98979591846</v>
+      </c>
+      <c r="B62">
+        <v>38303.574000000001</v>
+      </c>
+      <c r="C62">
+        <v>3.8304</v>
+      </c>
+      <c r="D62" s="13">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="E62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f>B63/D63</f>
+        <v>1077265.9405940594</v>
+      </c>
+      <c r="B63">
+        <v>32641.157999999999</v>
+      </c>
+      <c r="C63" s="11">
+        <v>3.2641</v>
+      </c>
+      <c r="D63" s="13">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f>B64/D64</f>
+        <v>1128093.0363036303</v>
+      </c>
+      <c r="B64">
+        <v>34181.218999999997</v>
+      </c>
+      <c r="C64">
+        <v>3.4180999999999999</v>
+      </c>
+      <c r="D64" s="13">
+        <v>3.0299999999999997E-2</v>
+      </c>
+      <c r="E64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f>B65/D65</f>
+        <v>1129417.5477707007</v>
+      </c>
+      <c r="B65">
+        <v>35463.711000000003</v>
+      </c>
+      <c r="C65">
+        <v>3.5464000000000002</v>
+      </c>
+      <c r="D65" s="13">
+        <v>3.1400000000000004E-2</v>
+      </c>
+      <c r="E65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f>B66/D66</f>
+        <v>1384820.4791666667</v>
+      </c>
+      <c r="B66">
+        <v>66471.383000000002</v>
+      </c>
+      <c r="C66" s="11">
+        <v>6.6471</v>
+      </c>
+      <c r="D66" s="13">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E66" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f>B67/D67</f>
+        <v>1486832.0091324202</v>
+      </c>
+      <c r="B67">
+        <v>32561.620999999999</v>
+      </c>
+      <c r="C67" s="11">
+        <v>3.2562000000000002</v>
+      </c>
+      <c r="D67" s="13">
+        <v>2.1899999999999999E-2</v>
+      </c>
+      <c r="E67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="B2:K18" xr:uid="{E1108626-858A-4027-BC1B-7377445CA427}"/>
+  <autoFilter ref="A2:G67" xr:uid="{A1C92FFF-D1FD-47B8-800D-712537A126E1}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G67">
+      <sortCondition ref="A2:A67"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -6083,10 +7980,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6185,486 +8082,6 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>0.81667000000000001</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0.81444000000000005</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.81667000000000001</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.81444000000000005</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.79727000000000003</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.81222000000000005</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.61973999999999996</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.79727000000000003</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.60111000000000003</v>
-      </c>
-      <c r="G7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.73</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.52297000000000005</v>
-      </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.72777999999999998</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.46516999999999997</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.72777999999999998</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.1133</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0.72333000000000003</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="1">
-        <v>4.2900000000000001E-2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.72111000000000003</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>0.70667000000000002</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0.69333</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0.61973999999999996</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>0.61602000000000001</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0.61231000000000002</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0.60133999999999999</v>
-      </c>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.60111000000000003</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>0.59777999999999998</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>0.52297000000000005</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>0.52175000000000005</v>
-      </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>0.51415</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>0.50927999999999995</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>0.46516999999999997</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>0.45695000000000002</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>0.43382999999999999</v>
-      </c>
-      <c r="B27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>0.40998000000000001</v>
-      </c>
-      <c r="B28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>0.1133</v>
-      </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>0.1105</v>
-      </c>
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>0.1099</v>
-      </c>
-      <c r="B31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>4.2900000000000001E-2</v>
-      </c>
-      <c r="B32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>3.4299999999999997E-2</v>
-      </c>
-      <c r="B33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>2.5399999999999999E-2</v>
-      </c>
-      <c r="B34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A2:C34" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C34">
-      <sortCondition descending="1" ref="A2:A34"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6695,7 +8112,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -6710,7 +8127,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -6735,7 +8152,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added time indicator row to stats
</commit_message>
<xml_diff>
--- a/stats_workbook.xlsx
+++ b/stats_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dawson\Learning\College\Spring 2023\ISSII\ISSII_Group3Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E442A9-686D-4130-9605-331200EBD0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FF97F4-CE88-4967-BEAA-E0EF772CF136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Stats" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">NAR_NN!$B$2:$K$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NN_NoLSTM!$B$2:$M$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Raw Stats'!$A$26:$E$42</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">RegressionLearner!$A$1:$G$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">RegressionLearner!$A$1:$H$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">seq!$A$1:$A$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="128">
   <si>
     <t>LSTM_Multichannel</t>
   </si>
@@ -1453,6 +1453,9 @@
   </si>
   <si>
     <t>Bit Penalty per Fraction Correctly Predicted</t>
+  </si>
+  <si>
+    <t>time predictor</t>
   </si>
 </sst>
 </file>
@@ -6356,24 +6359,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B9182A-1D61-4B81-884F-470869407FBE}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.05078125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83984375" style="19" customWidth="1"/>
-    <col min="7" max="7" width="8.83984375" style="23" customWidth="1"/>
+    <col min="1" max="1" width="10.47265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.3671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83984375" style="19" customWidth="1"/>
+    <col min="8" max="8" width="8.83984375" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -6381,273 +6385,304 @@
         <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="26">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G2,"penalty: "), " bits"))</f>
+      <c r="C2" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="26">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(H2,"penalty: "), " bits"))</f>
         <v>2193.645</v>
       </c>
-      <c r="D2" s="20">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G2,"bits (")," bits"))</f>
+      <c r="E2" s="20">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(H2,"bits (")," bits"))</f>
         <v>2.3041999999999998</v>
       </c>
-      <c r="E2" s="25">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G2,"predicted "),"% of")/100)</f>
+      <c r="F2" s="25">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(H2,"predicted "),"% of")/100)</f>
         <v>0.85714000000000001</v>
       </c>
-      <c r="F2" s="19">
-        <f>D2/E2</f>
+      <c r="G2" s="19">
+        <f>E2/F2</f>
         <v>2.6882422941409803</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="H2" s="24" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="26">
-        <f t="shared" ref="C3:C10" si="0">_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G3,"penalty: "), " bits"))</f>
+      <c r="C3" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="26">
+        <f t="shared" ref="D3:D10" si="0">_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(H3,"penalty: "), " bits"))</f>
         <v>2672.817</v>
       </c>
-      <c r="D3" s="20">
-        <f t="shared" ref="D3:D10" si="1">_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G3,"bits (")," bits"))</f>
+      <c r="E3" s="20">
+        <f t="shared" ref="E3:E10" si="1">_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(H3,"bits (")," bits"))</f>
         <v>2.9698000000000002</v>
       </c>
-      <c r="E3" s="25">
-        <f t="shared" ref="E3:E10" si="2">_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G3,"predicted "),"% of")/100)</f>
+      <c r="F3" s="25">
+        <f t="shared" ref="F3:F10" si="2">_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(H3,"predicted "),"% of")/100)</f>
         <v>0.81555999999999995</v>
       </c>
-      <c r="F3" s="19">
-        <f t="shared" ref="F3:F10" si="3">D3/E3</f>
+      <c r="G3" s="19">
+        <f t="shared" ref="G3:G10" si="3">E3/F3</f>
         <v>3.6414242974152735</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="H3" s="23" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="26">
         <f t="shared" si="0"/>
         <v>3189.7910000000002</v>
       </c>
-      <c r="D4" s="20">
+      <c r="E4" s="20">
         <f t="shared" si="1"/>
         <v>3.5442</v>
       </c>
-      <c r="E4" s="25">
+      <c r="F4" s="25">
         <f t="shared" si="2"/>
         <v>0.77666999999999997</v>
       </c>
-      <c r="F4" s="19">
+      <c r="G4" s="19">
         <f t="shared" si="3"/>
         <v>4.5633280543860328</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="H4" s="23" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="26">
         <f t="shared" si="0"/>
         <v>8125.2569999999996</v>
       </c>
-      <c r="D5" s="20">
+      <c r="E5" s="20">
         <f t="shared" si="1"/>
         <v>2.4719000000000002</v>
       </c>
-      <c r="E5" s="25">
+      <c r="F5" s="25">
         <f t="shared" si="2"/>
         <v>0.44447999999999999</v>
       </c>
-      <c r="F5" s="19">
+      <c r="G5" s="19">
         <f t="shared" si="3"/>
         <v>5.5613300935925132</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="H5" s="23" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="26">
         <f t="shared" si="0"/>
         <v>22996.685000000001</v>
       </c>
-      <c r="D6" s="20">
+      <c r="E6" s="20">
         <f t="shared" si="1"/>
         <v>6.9962999999999997</v>
       </c>
-      <c r="E6" s="25">
+      <c r="F6" s="25">
         <f t="shared" si="2"/>
         <v>0.50927999999999995</v>
       </c>
-      <c r="F6" s="19">
+      <c r="G6" s="19">
         <f t="shared" si="3"/>
         <v>13.737629594721961</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="23" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="26">
         <f t="shared" si="0"/>
         <v>18489.948</v>
       </c>
-      <c r="D7" s="20">
+      <c r="E7" s="20">
         <f t="shared" si="1"/>
         <v>3.2702</v>
       </c>
-      <c r="E7" s="25">
+      <c r="F7" s="25">
         <f t="shared" si="2"/>
         <v>0.17651</v>
       </c>
-      <c r="F7" s="19">
+      <c r="G7" s="19">
         <f t="shared" si="3"/>
         <v>18.526995637640926</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="H7" s="23" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="26">
         <f t="shared" si="0"/>
         <v>29146.080000000002</v>
       </c>
-      <c r="D8" s="20">
+      <c r="E8" s="20">
         <f t="shared" si="1"/>
         <v>2.9146000000000001</v>
       </c>
-      <c r="E8" s="25">
+      <c r="F8" s="25">
         <f t="shared" si="2"/>
         <v>0.17630000000000001</v>
       </c>
-      <c r="F8" s="19">
+      <c r="G8" s="19">
         <f t="shared" si="3"/>
         <v>16.532047646057855</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="H8" s="23" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="26">
         <f t="shared" si="0"/>
         <v>33684.972999999998</v>
       </c>
-      <c r="D9" s="20">
+      <c r="E9" s="20">
         <f t="shared" si="1"/>
         <v>3.3685</v>
       </c>
-      <c r="E9" s="25">
+      <c r="F9" s="25">
         <f t="shared" si="2"/>
         <v>0.11459999999999999</v>
       </c>
-      <c r="F9" s="19">
+      <c r="G9" s="19">
         <f t="shared" si="3"/>
         <v>29.393542757417105</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="H9" s="23" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="26">
         <f t="shared" si="0"/>
         <v>36504.053999999996</v>
       </c>
-      <c r="D10" s="20">
+      <c r="E10" s="20">
         <f t="shared" si="1"/>
         <v>3.6503999999999999</v>
       </c>
-      <c r="E10" s="25">
+      <c r="F10" s="25">
         <f t="shared" si="2"/>
         <v>9.0499999999999997E-2</v>
       </c>
-      <c r="F10" s="19">
+      <c r="G10" s="19">
         <f t="shared" si="3"/>
         <v>40.335911602209947</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="H10" s="23" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="19"/>
       <c r="B11" s="22"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G21" xr:uid="{84B9182A-1D61-4B81-884F-470869407FBE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
-      <sortCondition ref="F1:F21"/>
+  <autoFilter ref="A1:H21" xr:uid="{84B9182A-1D61-4B81-884F-470869407FBE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H21">
+      <sortCondition ref="G1:G21"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6659,8 +6694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C92FFF-D1FD-47B8-800D-712537A126E1}">
   <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6714,25 +6749,28 @@
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <f>C3/D3</f>
-        <v>0.87301957673192243</v>
-      </c>
-      <c r="B3">
-        <v>712.35400000000004</v>
-      </c>
-      <c r="C3" s="11">
-        <v>0.74829999999999997</v>
-      </c>
-      <c r="D3" s="13">
+        <v>2.6882422941409803</v>
+      </c>
+      <c r="B3" s="26">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G3,"penalty: "), " bits"))</f>
+        <v>2193.645</v>
+      </c>
+      <c r="C3" s="20">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G3,"bits (")," bits"))</f>
+        <v>2.3041999999999998</v>
+      </c>
+      <c r="D3" s="25">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G3,"predicted "),"% of")/100)</f>
         <v>0.85714000000000001</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
+      <c r="F3" t="s">
+        <v>114</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="13"/>
@@ -6742,25 +6780,28 @@
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <f>C4/D4</f>
-        <v>0.87301957673192243</v>
-      </c>
-      <c r="B4">
-        <v>712.35699999999997</v>
-      </c>
-      <c r="C4" s="11">
-        <v>0.74829999999999997</v>
-      </c>
-      <c r="D4" s="13">
-        <v>0.85714000000000001</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>106</v>
+        <v>3.6414242974152735</v>
+      </c>
+      <c r="B4" s="26">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G4,"penalty: "), " bits"))</f>
+        <v>2672.817</v>
+      </c>
+      <c r="C4" s="20">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G4,"bits (")," bits"))</f>
+        <v>2.9698000000000002</v>
+      </c>
+      <c r="D4" s="25">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G4,"predicted "),"% of")/100)</f>
+        <v>0.81555999999999995</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>119</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="13"/>
@@ -6769,25 +6810,28 @@
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f>C5/D5</f>
-        <v>1.0344706748122277</v>
-      </c>
-      <c r="B5">
-        <v>843.07299999999998</v>
-      </c>
-      <c r="C5">
-        <v>0.88560000000000005</v>
-      </c>
-      <c r="D5" s="13">
-        <v>0.85609000000000002</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>93</v>
+        <v>4.5633280543860328</v>
+      </c>
+      <c r="B5" s="26">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G5,"penalty: "), " bits"))</f>
+        <v>3189.7910000000002</v>
+      </c>
+      <c r="C5" s="20">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G5,"bits (")," bits"))</f>
+        <v>3.5442</v>
+      </c>
+      <c r="D5" s="25">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G5,"predicted "),"% of")/100)</f>
+        <v>0.77666999999999997</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>118</v>
       </c>
       <c r="L5" s="13"/>
       <c r="N5" s="3"/>
@@ -6795,25 +6839,28 @@
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <f>C6/D6</f>
-        <v>1.1254358823240507</v>
-      </c>
-      <c r="B6">
-        <v>824.899</v>
-      </c>
-      <c r="C6" s="11">
-        <v>0.91659999999999997</v>
-      </c>
-      <c r="D6" s="13">
-        <v>0.81444000000000005</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>53</v>
+        <v>5.5613300935925132</v>
+      </c>
+      <c r="B6" s="26">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G6,"penalty: "), " bits"))</f>
+        <v>8125.2569999999996</v>
+      </c>
+      <c r="C6" s="20">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G6,"bits (")," bits"))</f>
+        <v>2.4719000000000002</v>
+      </c>
+      <c r="D6" s="25">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G6,"predicted "),"% of")/100)</f>
+        <v>0.44447999999999999</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="L6" s="13"/>
       <c r="N6" s="3"/>
@@ -6821,25 +6868,28 @@
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <f>C7/D7</f>
-        <v>1.1254358823240507</v>
-      </c>
-      <c r="B7">
-        <v>824.94299999999998</v>
-      </c>
-      <c r="C7" s="11">
-        <v>0.91659999999999997</v>
-      </c>
-      <c r="D7" s="13">
-        <v>0.81444000000000005</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>52</v>
+        <v>13.737629594721961</v>
+      </c>
+      <c r="B7" s="26">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G7,"penalty: "), " bits"))</f>
+        <v>22996.685000000001</v>
+      </c>
+      <c r="C7" s="20">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G7,"bits (")," bits"))</f>
+        <v>6.9962999999999997</v>
+      </c>
+      <c r="D7" s="25">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G7,"predicted "),"% of")/100)</f>
+        <v>0.50927999999999995</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="L7" s="13"/>
       <c r="N7" s="3"/>
@@ -6847,25 +6897,28 @@
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <f>C8/D8</f>
-        <v>1.1261586687401275</v>
-      </c>
-      <c r="B8">
-        <v>827.71799999999996</v>
-      </c>
-      <c r="C8" s="11">
-        <v>0.91969999999999996</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0.81667000000000001</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>51</v>
+        <v>16.532047646057855</v>
+      </c>
+      <c r="B8" s="26">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G8,"penalty: "), " bits"))</f>
+        <v>29146.080000000002</v>
+      </c>
+      <c r="C8" s="20">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G8,"bits (")," bits"))</f>
+        <v>2.9146000000000001</v>
+      </c>
+      <c r="D8" s="25">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G8,"predicted "),"% of")/100)</f>
+        <v>0.17630000000000001</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>124</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="13"/>
@@ -6874,25 +6927,28 @@
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <f>C9/D9</f>
-        <v>1.126648462659336</v>
-      </c>
-      <c r="B9">
-        <v>828.05100000000004</v>
-      </c>
-      <c r="C9">
-        <v>0.92010000000000003</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.81667000000000001</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>97</v>
+        <v>18.526995637640926</v>
+      </c>
+      <c r="B9" s="26">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G9,"penalty: "), " bits"))</f>
+        <v>18489.948</v>
+      </c>
+      <c r="C9" s="20">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G9,"bits (")," bits"))</f>
+        <v>3.2702</v>
+      </c>
+      <c r="D9" s="25">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G9,"predicted "),"% of")/100)</f>
+        <v>0.17651</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>122</v>
       </c>
       <c r="K9" s="11"/>
       <c r="L9" s="13"/>
@@ -6901,25 +6957,28 @@
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <f>C10/D10</f>
-        <v>1.1804076265614729</v>
-      </c>
-      <c r="B10">
-        <v>854.60299999999995</v>
-      </c>
-      <c r="C10" s="11">
-        <v>0.89770000000000005</v>
-      </c>
-      <c r="D10" s="13">
-        <v>0.76049999999999995</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>102</v>
+        <v>29.393542757417105</v>
+      </c>
+      <c r="B10" s="26">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G10,"penalty: "), " bits"))</f>
+        <v>33684.972999999998</v>
+      </c>
+      <c r="C10" s="20">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G10,"bits (")," bits"))</f>
+        <v>3.3685</v>
+      </c>
+      <c r="D10" s="25">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G10,"predicted "),"% of")/100)</f>
+        <v>0.11459999999999999</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>123</v>
       </c>
       <c r="L10" s="13"/>
       <c r="N10" s="3"/>
@@ -6927,109 +6986,112 @@
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <f>C11/D11</f>
-        <v>1.263006182282514</v>
-      </c>
-      <c r="B11">
-        <v>951.06399999999996</v>
-      </c>
-      <c r="C11" s="11">
-        <v>0.999</v>
-      </c>
-      <c r="D11" s="13">
-        <v>0.79096999999999995</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>60</v>
+        <v>40.335911602209947</v>
+      </c>
+      <c r="B11" s="26">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G11,"penalty: "), " bits"))</f>
+        <v>36504.053999999996</v>
+      </c>
+      <c r="C11" s="20">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G11,"bits (")," bits"))</f>
+        <v>3.6503999999999999</v>
+      </c>
+      <c r="D11" s="25">
+        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G11,"predicted "),"% of")/100)</f>
+        <v>9.0499999999999997E-2</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <f>C12/D12</f>
-        <v>1.2631125161661156</v>
-      </c>
-      <c r="B12" s="3">
-        <v>1004.174</v>
-      </c>
-      <c r="C12">
-        <v>1.0548</v>
+        <v>0.87301957673192243</v>
+      </c>
+      <c r="B12">
+        <v>712.35400000000004</v>
+      </c>
+      <c r="C12" s="11">
+        <v>0.74829999999999997</v>
       </c>
       <c r="D12" s="13">
-        <v>0.83508000000000004</v>
+        <v>0.85714000000000001</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <f>C13/D13</f>
-        <v>1.3162734807984697</v>
+        <v>0.87301957673192243</v>
       </c>
       <c r="B13">
-        <v>966.12300000000005</v>
-      </c>
-      <c r="C13">
-        <v>1.0734999999999999</v>
+        <v>712.35699999999997</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0.74829999999999997</v>
       </c>
       <c r="D13" s="13">
-        <v>0.81555999999999995</v>
+        <v>0.85714000000000001</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <f>C14/D14</f>
-        <v>1.3305276788604725</v>
+        <v>1.1254358823240507</v>
       </c>
       <c r="B14">
-        <v>1056.3889999999999</v>
-      </c>
-      <c r="C14">
-        <v>1.1096999999999999</v>
+        <v>824.899</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.91659999999999997</v>
       </c>
       <c r="D14" s="13">
-        <v>0.83403000000000005</v>
+        <v>0.81444000000000005</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <f>C15/D15</f>
-        <v>1.6664210991601589</v>
+        <v>1.1254358823240507</v>
       </c>
       <c r="B15">
-        <v>1221.4570000000001</v>
-      </c>
-      <c r="C15">
-        <v>1.3572</v>
+        <v>824.94299999999998</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0.91659999999999997</v>
       </c>
       <c r="D15" s="13">
         <v>0.81444000000000005</v>
@@ -7038,1420 +7100,1393 @@
         <v>6</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <f>C16/D16</f>
-        <v>1.6760278589081103</v>
+        <v>1.1261586687401275</v>
       </c>
       <c r="B16">
-        <v>1141.374</v>
-      </c>
-      <c r="C16">
-        <v>1.2682</v>
+        <v>827.71799999999996</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0.91969999999999996</v>
       </c>
       <c r="D16" s="13">
-        <v>0.75667000000000006</v>
+        <v>0.81667000000000001</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <f>C17/D17</f>
-        <v>1.6842247433819555</v>
+        <v>1.126648462659336</v>
       </c>
       <c r="B17">
-        <v>1234.5609999999999</v>
-      </c>
-      <c r="C17" s="11">
-        <v>1.3716999999999999</v>
-      </c>
-      <c r="D17" s="13">
-        <v>0.81444000000000005</v>
+        <v>828.05100000000004</v>
+      </c>
+      <c r="C17">
+        <v>0.92010000000000003</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.81667000000000001</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <f>C18/D18</f>
-        <v>1.6937500000000001</v>
+        <v>1.1804076265614729</v>
       </c>
       <c r="B18">
-        <v>1097.5930000000001</v>
+        <v>854.60299999999995</v>
       </c>
       <c r="C18" s="11">
-        <v>1.2195</v>
+        <v>0.89770000000000005</v>
       </c>
       <c r="D18" s="13">
-        <v>0.72</v>
+        <v>0.76049999999999995</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <f>C19/D19</f>
-        <v>1.8106828249910891</v>
+        <v>2.9311204975554594</v>
       </c>
       <c r="B19">
-        <v>1280.1980000000001</v>
+        <v>10263.27</v>
       </c>
       <c r="C19">
-        <v>1.4224000000000001</v>
-      </c>
-      <c r="D19" s="13">
-        <v>0.78556000000000004</v>
+        <v>1.7625999999999999</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.60133999999999999</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <f>C20/D20</f>
-        <v>1.8124819931676932</v>
+        <v>2.9688695247281074</v>
       </c>
       <c r="B20">
-        <v>1188.9880000000001</v>
+        <v>10093.81</v>
       </c>
       <c r="C20" s="11">
-        <v>1.3210999999999999</v>
+        <v>1.7853000000000001</v>
       </c>
       <c r="D20" s="13">
-        <v>0.72889000000000004</v>
+        <v>0.60133999999999999</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <f>C21/D21</f>
-        <v>1.9880729302020215</v>
+        <v>2.9904879103335884</v>
       </c>
       <c r="B21">
-        <v>1308.1220000000001</v>
+        <v>10167.869000000001</v>
       </c>
       <c r="C21">
-        <v>1.4535</v>
-      </c>
-      <c r="D21" s="13">
-        <v>0.73111000000000004</v>
+        <v>1.7983</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.60133999999999999</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <f>C22/D22</f>
-        <v>2.0629999039635609</v>
+        <v>3.0185918116207135</v>
       </c>
       <c r="B22">
-        <v>1353.373</v>
-      </c>
-      <c r="C22" s="11">
-        <v>1.5037</v>
-      </c>
-      <c r="D22" s="13">
-        <v>0.72889000000000004</v>
+        <v>10263.27</v>
+      </c>
+      <c r="C22">
+        <v>1.8151999999999999</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.60133999999999999</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <f>C23/D23</f>
-        <v>2.1291021423413303</v>
+        <v>3.3561105874960733</v>
       </c>
       <c r="B23">
-        <v>1432.91</v>
-      </c>
-      <c r="C23">
-        <v>1.5921000000000001</v>
+        <v>5618.3040000000001</v>
+      </c>
+      <c r="C23" s="11">
+        <v>1.7092000000000001</v>
       </c>
       <c r="D23" s="13">
-        <v>0.74778000000000011</v>
+        <v>0.50927999999999995</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <f>C24/D24</f>
-        <v>2.1610958904109587</v>
+        <v>3.3680882814954449</v>
       </c>
       <c r="B24">
-        <v>1419.8810000000001</v>
+        <v>5638.2669999999998</v>
       </c>
       <c r="C24" s="11">
-        <v>1.5775999999999999</v>
+        <v>1.7153</v>
       </c>
       <c r="D24" s="13">
-        <v>0.73</v>
+        <v>0.50927999999999995</v>
       </c>
       <c r="E24" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <f>C25/D25</f>
-        <v>2.3538706752040452</v>
+        <v>4.0695745826602048</v>
       </c>
       <c r="B25">
-        <v>1541.8119999999999</v>
+        <v>6210.174</v>
       </c>
       <c r="C25" s="11">
-        <v>1.7131000000000001</v>
+        <v>1.8893</v>
       </c>
       <c r="D25" s="13">
-        <v>0.72777999999999998</v>
+        <v>0.46425</v>
       </c>
       <c r="E25" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <f>C26/D26</f>
-        <v>2.5613698630136987</v>
+        <v>4.0997325511172464</v>
       </c>
       <c r="B26">
-        <v>1682.8320000000001</v>
+        <v>6247.8739999999998</v>
       </c>
       <c r="C26" s="11">
-        <v>1.8697999999999999</v>
+        <v>1.9008</v>
       </c>
       <c r="D26" s="13">
-        <v>0.73</v>
+        <v>0.46364</v>
       </c>
       <c r="E26" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <f>C27/D27</f>
-        <v>2.5676386696574451</v>
+        <v>4.1141589522631286</v>
       </c>
       <c r="B27">
-        <v>1668.934</v>
+        <v>6340.0420000000004</v>
       </c>
       <c r="C27" s="11">
-        <v>1.8544</v>
+        <v>1.9288000000000001</v>
       </c>
       <c r="D27" s="13">
-        <v>0.72221999999999997</v>
+        <v>0.46882000000000001</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <f>C28/D28</f>
-        <v>2.6882422941409803</v>
-      </c>
-      <c r="B28" s="26">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G28,"penalty: "), " bits"))</f>
-        <v>2193.645</v>
-      </c>
-      <c r="C28" s="20">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G28,"bits (")," bits"))</f>
-        <v>2.3041999999999998</v>
-      </c>
-      <c r="D28" s="25">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G28,"predicted "),"% of")/100)</f>
-        <v>0.85714000000000001</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" t="s">
-        <v>114</v>
+        <v>27.716404886561957</v>
+      </c>
+      <c r="B28">
+        <v>31763.324000000001</v>
+      </c>
+      <c r="C28" s="11">
+        <v>3.1762999999999999</v>
+      </c>
+      <c r="D28" s="13">
+        <v>0.11459999999999999</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>117</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <f>C29/D29</f>
-        <v>2.7587594354046963</v>
+        <v>148.68493150684932</v>
       </c>
       <c r="B29">
-        <v>9691.6569999999992</v>
-      </c>
-      <c r="C29">
-        <v>1.7141</v>
+        <v>32561.620999999999</v>
+      </c>
+      <c r="C29" s="11">
+        <v>3.2562000000000002</v>
       </c>
       <c r="D29" s="13">
-        <v>0.62133000000000005</v>
+        <v>2.1899999999999999E-2</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <f>C30/D30</f>
-        <v>2.7636970054198593</v>
+        <v>1.263006182282514</v>
       </c>
       <c r="B30">
-        <v>1730.1410000000001</v>
+        <v>951.06399999999996</v>
       </c>
       <c r="C30" s="11">
-        <v>1.9224000000000001</v>
+        <v>0.999</v>
       </c>
       <c r="D30" s="13">
-        <v>0.69559000000000004</v>
+        <v>0.79096999999999995</v>
       </c>
       <c r="E30" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <f>C31/D31</f>
-        <v>2.7684724271561301</v>
+        <v>1.6937500000000001</v>
       </c>
       <c r="B31">
-        <v>9638.1049999999996</v>
+        <v>1097.5930000000001</v>
       </c>
       <c r="C31" s="11">
-        <v>1.7074</v>
+        <v>1.2195</v>
       </c>
       <c r="D31" s="13">
-        <v>0.61673</v>
+        <v>0.72</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <f>C32/D32</f>
-        <v>2.7763249792908535</v>
+        <v>1.8124819931676932</v>
       </c>
       <c r="B32">
-        <v>9664.6039999999994</v>
+        <v>1188.9880000000001</v>
       </c>
       <c r="C32" s="11">
-        <v>1.7093</v>
+        <v>1.3210999999999999</v>
       </c>
       <c r="D32" s="13">
-        <v>0.61567000000000005</v>
+        <v>0.72889000000000004</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <f>C33/D33</f>
-        <v>2.8381666666666669</v>
+        <v>2.0629999039635609</v>
       </c>
       <c r="B33">
-        <v>1532.616</v>
+        <v>1353.373</v>
       </c>
       <c r="C33" s="11">
-        <v>1.7029000000000001</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0.6</v>
+        <v>1.5037</v>
+      </c>
+      <c r="D33" s="13">
+        <v>0.72889000000000004</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <f>C34/D34</f>
-        <v>2.8493360738638214</v>
-      </c>
-      <c r="B34" s="3">
-        <v>9875.56</v>
-      </c>
-      <c r="C34">
-        <v>1.7466999999999999</v>
+        <v>2.1610958904109587</v>
+      </c>
+      <c r="B34">
+        <v>1419.8810000000001</v>
+      </c>
+      <c r="C34" s="11">
+        <v>1.5775999999999999</v>
       </c>
       <c r="D34" s="13">
-        <v>0.61302000000000001</v>
+        <v>0.73</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <f>C35/D35</f>
-        <v>2.8629537430240317</v>
+        <v>2.3538706752040452</v>
       </c>
       <c r="B35">
-        <v>9948.6350000000002</v>
-      </c>
-      <c r="C35">
-        <v>1.7596000000000001</v>
+        <v>1541.8119999999999</v>
+      </c>
+      <c r="C35" s="11">
+        <v>1.7131000000000001</v>
       </c>
       <c r="D35" s="13">
-        <v>0.61460999999999999</v>
+        <v>0.72777999999999998</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <f>C36/D36</f>
-        <v>2.9311204975554594</v>
+        <v>2.5613698630136987</v>
       </c>
       <c r="B36">
-        <v>10263.27</v>
-      </c>
-      <c r="C36">
-        <v>1.7625999999999999</v>
-      </c>
-      <c r="D36" s="1">
-        <v>0.60133999999999999</v>
+        <v>1682.8320000000001</v>
+      </c>
+      <c r="C36" s="11">
+        <v>1.8697999999999999</v>
+      </c>
+      <c r="D36" s="13">
+        <v>0.73</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <f>C37/D37</f>
-        <v>2.9370492125018397</v>
+        <v>2.5676386696574451</v>
       </c>
       <c r="B37">
-        <v>10153.495000000001</v>
+        <v>1668.934</v>
       </c>
       <c r="C37" s="11">
-        <v>1.7958000000000001</v>
+        <v>1.8544</v>
       </c>
       <c r="D37" s="13">
-        <v>0.61143000000000003</v>
+        <v>0.72221999999999997</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <f>C38/D38</f>
-        <v>2.9663378387034784</v>
+        <v>2.7636970054198593</v>
       </c>
       <c r="B38">
-        <v>1667.097</v>
+        <v>1730.1410000000001</v>
       </c>
       <c r="C38" s="11">
-        <v>1.8523000000000001</v>
-      </c>
-      <c r="D38" s="1">
-        <v>0.62444</v>
+        <v>1.9224000000000001</v>
+      </c>
+      <c r="D38" s="13">
+        <v>0.69559000000000004</v>
       </c>
       <c r="E38" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <f>C39/D39</f>
-        <v>2.9688695247281074</v>
+        <v>2.8381666666666669</v>
       </c>
       <c r="B39">
-        <v>10093.81</v>
+        <v>1532.616</v>
       </c>
       <c r="C39" s="11">
-        <v>1.7853000000000001</v>
-      </c>
-      <c r="D39" s="13">
-        <v>0.60133999999999999</v>
+        <v>1.7029000000000001</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.6</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <f>C40/D40</f>
-        <v>2.9904879103335884</v>
+        <v>2.9663378387034784</v>
       </c>
       <c r="B40">
-        <v>10167.869000000001</v>
-      </c>
-      <c r="C40">
-        <v>1.7983</v>
+        <v>1667.097</v>
+      </c>
+      <c r="C40" s="11">
+        <v>1.8523000000000001</v>
       </c>
       <c r="D40" s="1">
-        <v>0.60133999999999999</v>
+        <v>0.62444</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <f>C41/D41</f>
-        <v>3.0185918116207135</v>
+        <v>3.1784738632745069</v>
       </c>
       <c r="B41">
-        <v>10263.27</v>
-      </c>
-      <c r="C41">
-        <v>1.8151999999999999</v>
-      </c>
-      <c r="D41" s="1">
-        <v>0.60133999999999999</v>
+        <v>1706.893</v>
+      </c>
+      <c r="C41" s="11">
+        <v>1.8965000000000001</v>
+      </c>
+      <c r="D41" s="13">
+        <v>0.59667000000000003</v>
       </c>
       <c r="E41" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <f>C42/D42</f>
-        <v>3.1005528614827251</v>
+        <v>3.1914291893330673</v>
       </c>
       <c r="B42">
-        <v>5401.1049999999996</v>
-      </c>
-      <c r="C42">
-        <v>1.6432</v>
+        <v>1726.5519999999999</v>
+      </c>
+      <c r="C42" s="11">
+        <v>1.9184000000000001</v>
       </c>
       <c r="D42" s="13">
-        <v>0.52997000000000005</v>
+        <v>0.60111000000000003</v>
       </c>
       <c r="E42" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <f>C43/D43</f>
-        <v>3.1770464845019788</v>
+        <v>4.3007406758118938</v>
       </c>
       <c r="B43">
-        <v>5461.3530000000001</v>
+        <v>6451.2250000000004</v>
       </c>
       <c r="C43" s="11">
-        <v>1.6615</v>
+        <v>1.9625999999999999</v>
       </c>
       <c r="D43" s="13">
-        <v>0.52297000000000005</v>
+        <v>0.45634000000000002</v>
       </c>
       <c r="E43" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <f>C44/D44</f>
-        <v>3.1784738632745069</v>
+        <v>4.7426937005512873</v>
       </c>
       <c r="B44">
-        <v>1706.893</v>
+        <v>6758.4920000000002</v>
       </c>
       <c r="C44" s="11">
-        <v>1.8965000000000001</v>
+        <v>2.0560999999999998</v>
       </c>
       <c r="D44" s="13">
-        <v>0.59667000000000003</v>
+        <v>0.43353000000000003</v>
       </c>
       <c r="E44" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <f>C45/D45</f>
-        <v>3.1914291893330673</v>
+        <v>7.5206107615005608</v>
       </c>
       <c r="B45">
-        <v>1726.5519999999999</v>
+        <v>17432.940999999999</v>
       </c>
       <c r="C45" s="11">
-        <v>1.9184000000000001</v>
+        <v>3.0832999999999999</v>
       </c>
       <c r="D45" s="13">
-        <v>0.60111000000000003</v>
+        <v>0.40998000000000001</v>
       </c>
       <c r="E45" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <f>C46/D46</f>
-        <v>3.2118477159301677</v>
+        <v>28.77956989247312</v>
       </c>
       <c r="B46">
-        <v>5521.0739999999996</v>
+        <v>32117.952000000001</v>
       </c>
       <c r="C46" s="11">
-        <v>1.6797</v>
+        <v>3.2118000000000002</v>
       </c>
       <c r="D46" s="13">
-        <v>0.52297000000000005</v>
+        <v>0.1116</v>
       </c>
       <c r="E46" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <f>C47/D47</f>
-        <v>3.214183037853378</v>
+        <v>107.72607260726072</v>
       </c>
       <c r="B47">
-        <v>5512.2709999999997</v>
-      </c>
-      <c r="C47">
-        <v>1.677</v>
+        <v>32641.157999999999</v>
+      </c>
+      <c r="C47" s="11">
+        <v>3.2641</v>
       </c>
       <c r="D47" s="13">
-        <v>0.52175000000000005</v>
+        <v>3.0300000000000001E-2</v>
       </c>
       <c r="E47" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <f>C48/D48</f>
-        <v>3.2789510053427264</v>
+        <v>1.0344706748122277</v>
       </c>
       <c r="B48">
-        <v>1750.95</v>
-      </c>
-      <c r="C48" s="11">
-        <v>1.9455</v>
+        <v>843.07299999999998</v>
+      </c>
+      <c r="C48">
+        <v>0.88560000000000005</v>
       </c>
       <c r="D48" s="13">
-        <v>0.59333000000000002</v>
+        <v>0.85609000000000002</v>
       </c>
       <c r="E48" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <f>C49/D49</f>
-        <v>3.3561105874960733</v>
-      </c>
-      <c r="B49">
-        <v>5618.3040000000001</v>
-      </c>
-      <c r="C49" s="11">
-        <v>1.7092000000000001</v>
+        <v>1.2631125161661156</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1004.174</v>
+      </c>
+      <c r="C49">
+        <v>1.0548</v>
       </c>
       <c r="D49" s="13">
-        <v>0.50927999999999995</v>
+        <v>0.83508000000000004</v>
       </c>
       <c r="E49" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G49" s="24" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <f>C50/D50</f>
-        <v>3.3680882814954449</v>
+        <v>1.3162734807984697</v>
       </c>
       <c r="B50">
-        <v>5638.2669999999998</v>
-      </c>
-      <c r="C50" s="11">
-        <v>1.7153</v>
+        <v>966.12300000000005</v>
+      </c>
+      <c r="C50">
+        <v>1.0734999999999999</v>
       </c>
       <c r="D50" s="13">
-        <v>0.50927999999999995</v>
+        <v>0.81555999999999995</v>
       </c>
       <c r="E50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <f>C51/D51</f>
-        <v>3.6414242974152735</v>
-      </c>
-      <c r="B51" s="26">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G51,"penalty: "), " bits"))</f>
-        <v>2672.817</v>
-      </c>
-      <c r="C51" s="20">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G51,"bits (")," bits"))</f>
-        <v>2.9698000000000002</v>
-      </c>
-      <c r="D51" s="25">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G51,"predicted "),"% of")/100)</f>
-        <v>0.81555999999999995</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F51" t="s">
-        <v>114</v>
-      </c>
-      <c r="G51" s="23" t="s">
-        <v>119</v>
+        <v>1.3305276788604725</v>
+      </c>
+      <c r="B51">
+        <v>1056.3889999999999</v>
+      </c>
+      <c r="C51">
+        <v>1.1096999999999999</v>
+      </c>
+      <c r="D51" s="13">
+        <v>0.83403000000000005</v>
+      </c>
+      <c r="E51" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G51" s="24" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <f>C52/D52</f>
-        <v>4.0695745826602048</v>
+        <v>1.6664210991601589</v>
       </c>
       <c r="B52">
-        <v>6210.174</v>
-      </c>
-      <c r="C52" s="11">
-        <v>1.8893</v>
+        <v>1221.4570000000001</v>
+      </c>
+      <c r="C52">
+        <v>1.3572</v>
       </c>
       <c r="D52" s="13">
-        <v>0.46425</v>
+        <v>0.81444000000000005</v>
       </c>
       <c r="E52" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <f>C53/D53</f>
-        <v>4.0997325511172464</v>
+        <v>1.6760278589081103</v>
       </c>
       <c r="B53">
-        <v>6247.8739999999998</v>
-      </c>
-      <c r="C53" s="11">
-        <v>1.9008</v>
+        <v>1141.374</v>
+      </c>
+      <c r="C53">
+        <v>1.2682</v>
       </c>
       <c r="D53" s="13">
-        <v>0.46364</v>
+        <v>0.75667000000000006</v>
       </c>
       <c r="E53" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G53" s="24" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <f>C54/D54</f>
-        <v>4.1141589522631286</v>
+        <v>1.6842247433819555</v>
       </c>
       <c r="B54">
-        <v>6340.0420000000004</v>
+        <v>1234.5609999999999</v>
       </c>
       <c r="C54" s="11">
-        <v>1.9288000000000001</v>
+        <v>1.3716999999999999</v>
       </c>
       <c r="D54" s="13">
-        <v>0.46882000000000001</v>
+        <v>0.81444000000000005</v>
       </c>
       <c r="E54" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <f>C55/D55</f>
-        <v>4.3007406758118938</v>
+        <v>1.8106828249910891</v>
       </c>
       <c r="B55">
-        <v>6451.2250000000004</v>
-      </c>
-      <c r="C55" s="11">
-        <v>1.9625999999999999</v>
+        <v>1280.1980000000001</v>
+      </c>
+      <c r="C55">
+        <v>1.4224000000000001</v>
       </c>
       <c r="D55" s="13">
-        <v>0.45634000000000002</v>
+        <v>0.78556000000000004</v>
       </c>
       <c r="E55" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <f>C56/D56</f>
-        <v>4.5633280543860328</v>
-      </c>
-      <c r="B56" s="26">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G56,"penalty: "), " bits"))</f>
-        <v>3189.7910000000002</v>
-      </c>
-      <c r="C56" s="20">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G56,"bits (")," bits"))</f>
-        <v>3.5442</v>
-      </c>
-      <c r="D56" s="25">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G56,"predicted "),"% of")/100)</f>
-        <v>0.77666999999999997</v>
-      </c>
-      <c r="E56" s="19" t="s">
+        <v>1.9880729302020215</v>
+      </c>
+      <c r="B56">
+        <v>1308.1220000000001</v>
+      </c>
+      <c r="C56">
+        <v>1.4535</v>
+      </c>
+      <c r="D56" s="13">
+        <v>0.73111000000000004</v>
+      </c>
+      <c r="E56" t="s">
         <v>20</v>
       </c>
-      <c r="F56" t="s">
-        <v>114</v>
-      </c>
-      <c r="G56" s="23" t="s">
-        <v>118</v>
+      <c r="F56" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G56" s="24" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <f>C57/D57</f>
-        <v>4.7426937005512873</v>
+        <v>2.1291021423413303</v>
       </c>
       <c r="B57">
-        <v>6758.4920000000002</v>
-      </c>
-      <c r="C57" s="11">
-        <v>2.0560999999999998</v>
+        <v>1432.91</v>
+      </c>
+      <c r="C57">
+        <v>1.5921000000000001</v>
       </c>
       <c r="D57" s="13">
-        <v>0.43353000000000003</v>
+        <v>0.74778000000000011</v>
       </c>
       <c r="E57" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G57" s="24" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <f>C58/D58</f>
-        <v>5.5613300935925132</v>
-      </c>
-      <c r="B58" s="26">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G58,"penalty: "), " bits"))</f>
-        <v>8125.2569999999996</v>
-      </c>
-      <c r="C58" s="20">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G58,"bits (")," bits"))</f>
-        <v>2.4719000000000002</v>
-      </c>
-      <c r="D58" s="25">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G58,"predicted "),"% of")/100)</f>
-        <v>0.44447999999999999</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F58" t="s">
-        <v>114</v>
-      </c>
-      <c r="G58" s="23" t="s">
-        <v>120</v>
+        <v>2.7587594354046963</v>
+      </c>
+      <c r="B58">
+        <v>9691.6569999999992</v>
+      </c>
+      <c r="C58">
+        <v>1.7141</v>
+      </c>
+      <c r="D58" s="13">
+        <v>0.62133000000000005</v>
+      </c>
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G58" s="24" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <f>C59/D59</f>
-        <v>7.5206107615005608</v>
+        <v>2.7684724271561301</v>
       </c>
       <c r="B59">
-        <v>17432.940999999999</v>
+        <v>9638.1049999999996</v>
       </c>
       <c r="C59" s="11">
-        <v>3.0832999999999999</v>
+        <v>1.7074</v>
       </c>
       <c r="D59" s="13">
-        <v>0.40998000000000001</v>
+        <v>0.61673</v>
       </c>
       <c r="E59" t="s">
         <v>8</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <f>C60/D60</f>
-        <v>13.737629594721961</v>
-      </c>
-      <c r="B60" s="26">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G60,"penalty: "), " bits"))</f>
-        <v>22996.685000000001</v>
-      </c>
-      <c r="C60" s="20">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G60,"bits (")," bits"))</f>
-        <v>6.9962999999999997</v>
-      </c>
-      <c r="D60" s="25">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G60,"predicted "),"% of")/100)</f>
-        <v>0.50927999999999995</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F60" t="s">
-        <v>114</v>
-      </c>
-      <c r="G60" s="23" t="s">
-        <v>121</v>
+        <v>2.7763249792908535</v>
+      </c>
+      <c r="B60">
+        <v>9664.6039999999994</v>
+      </c>
+      <c r="C60" s="11">
+        <v>1.7093</v>
+      </c>
+      <c r="D60" s="13">
+        <v>0.61567000000000005</v>
+      </c>
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G60" s="24" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <f>C61/D61</f>
-        <v>16.532047646057855</v>
-      </c>
-      <c r="B61" s="26">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G61,"penalty: "), " bits"))</f>
-        <v>29146.080000000002</v>
-      </c>
-      <c r="C61" s="20">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G61,"bits (")," bits"))</f>
-        <v>2.9146000000000001</v>
-      </c>
-      <c r="D61" s="25">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G61,"predicted "),"% of")/100)</f>
-        <v>0.17630000000000001</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" t="s">
-        <v>114</v>
-      </c>
-      <c r="G61" s="23" t="s">
-        <v>124</v>
+        <v>2.8493360738638214</v>
+      </c>
+      <c r="B61" s="3">
+        <v>9875.56</v>
+      </c>
+      <c r="C61">
+        <v>1.7466999999999999</v>
+      </c>
+      <c r="D61" s="13">
+        <v>0.61302000000000001</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G61" s="24" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <f>C62/D62</f>
-        <v>18.526995637640926</v>
-      </c>
-      <c r="B62" s="26">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G62,"penalty: "), " bits"))</f>
-        <v>18489.948</v>
-      </c>
-      <c r="C62" s="20">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G62,"bits (")," bits"))</f>
-        <v>3.2702</v>
-      </c>
-      <c r="D62" s="25">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G62,"predicted "),"% of")/100)</f>
-        <v>0.17651</v>
-      </c>
-      <c r="E62" s="19" t="s">
+        <v>2.8629537430240317</v>
+      </c>
+      <c r="B62">
+        <v>9948.6350000000002</v>
+      </c>
+      <c r="C62">
+        <v>1.7596000000000001</v>
+      </c>
+      <c r="D62" s="13">
+        <v>0.61460999999999999</v>
+      </c>
+      <c r="E62" t="s">
         <v>8</v>
       </c>
-      <c r="F62" t="s">
-        <v>114</v>
-      </c>
-      <c r="G62" s="23" t="s">
-        <v>122</v>
+      <c r="F62" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G62" s="24" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <f>C63/D63</f>
-        <v>27.716404886561957</v>
+        <v>2.9370492125018397</v>
       </c>
       <c r="B63">
-        <v>31763.324000000001</v>
+        <v>10153.495000000001</v>
       </c>
       <c r="C63" s="11">
-        <v>3.1762999999999999</v>
+        <v>1.7958000000000001</v>
       </c>
       <c r="D63" s="13">
-        <v>0.11459999999999999</v>
+        <v>0.61143000000000003</v>
       </c>
       <c r="E63" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G63" s="24" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <f>C64/D64</f>
-        <v>28.062555066079295</v>
+        <v>3.1005528614827251</v>
       </c>
       <c r="B64">
-        <v>31850.853999999999</v>
+        <v>5401.1049999999996</v>
       </c>
       <c r="C64">
-        <v>3.1850999999999998</v>
+        <v>1.6432</v>
       </c>
       <c r="D64" s="13">
-        <v>0.11349999999999999</v>
+        <v>0.52997000000000005</v>
       </c>
       <c r="E64" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G64" s="24" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <f>C65/D65</f>
-        <v>28.307759372275502</v>
+        <v>3.1770464845019788</v>
       </c>
       <c r="B65">
-        <v>32469.059000000001</v>
-      </c>
-      <c r="C65">
-        <v>3.2469000000000001</v>
+        <v>5461.3530000000001</v>
+      </c>
+      <c r="C65" s="11">
+        <v>1.6615</v>
       </c>
       <c r="D65" s="13">
-        <v>0.1147</v>
+        <v>0.52297000000000005</v>
       </c>
       <c r="E65" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G65" s="24" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <f>C66/D66</f>
-        <v>28.310798946444251</v>
+        <v>3.2118477159301677</v>
       </c>
       <c r="B66">
-        <v>32246.17</v>
+        <v>5521.0739999999996</v>
       </c>
       <c r="C66" s="11">
-        <v>3.2246000000000001</v>
+        <v>1.6797</v>
       </c>
       <c r="D66" s="13">
-        <v>0.1139</v>
+        <v>0.52297000000000005</v>
       </c>
       <c r="E66" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G66" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <f>C67/D67</f>
-        <v>28.77956989247312</v>
+        <v>3.214183037853378</v>
       </c>
       <c r="B67">
-        <v>32117.952000000001</v>
-      </c>
-      <c r="C67" s="11">
-        <v>3.2118000000000002</v>
+        <v>5512.2709999999997</v>
+      </c>
+      <c r="C67">
+        <v>1.677</v>
       </c>
       <c r="D67" s="13">
-        <v>0.1116</v>
+        <v>0.52175000000000005</v>
       </c>
       <c r="E67" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G67" s="24" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <f>C68/D68</f>
-        <v>29.261187214611876</v>
+        <v>3.2789510053427264</v>
       </c>
       <c r="B68">
-        <v>32040.548999999999</v>
-      </c>
-      <c r="C68">
-        <v>3.2040999999999999</v>
+        <v>1750.95</v>
+      </c>
+      <c r="C68" s="11">
+        <v>1.9455</v>
       </c>
       <c r="D68" s="13">
-        <v>0.10949999999999999</v>
+        <v>0.59333000000000002</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G68" s="24" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <f>C69/D69</f>
-        <v>29.393542757417105</v>
-      </c>
-      <c r="B69" s="26">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G69,"penalty: "), " bits"))</f>
-        <v>33684.972999999998</v>
-      </c>
-      <c r="C69" s="20">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G69,"bits (")," bits"))</f>
-        <v>3.3685</v>
-      </c>
-      <c r="D69" s="25">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G69,"predicted "),"% of")/100)</f>
-        <v>0.11459999999999999</v>
-      </c>
-      <c r="E69" s="19" t="s">
+        <v>28.062555066079295</v>
+      </c>
+      <c r="B69">
+        <v>31850.853999999999</v>
+      </c>
+      <c r="C69">
+        <v>3.1850999999999998</v>
+      </c>
+      <c r="D69" s="13">
+        <v>0.11349999999999999</v>
+      </c>
+      <c r="E69" t="s">
         <v>10</v>
       </c>
-      <c r="F69" t="s">
-        <v>114</v>
-      </c>
-      <c r="G69" s="23" t="s">
-        <v>123</v>
+      <c r="F69" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G69" s="24" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <f>C70/D70</f>
-        <v>40.335911602209947</v>
-      </c>
-      <c r="B70" s="26">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G70,"penalty: "), " bits"))</f>
-        <v>36504.053999999996</v>
-      </c>
-      <c r="C70" s="20">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G70,"bits (")," bits"))</f>
-        <v>3.6503999999999999</v>
-      </c>
-      <c r="D70" s="25">
-        <f>_xlfn.NUMBERVALUE(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(G70,"predicted "),"% of")/100)</f>
-        <v>9.0499999999999997E-2</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="F70" t="s">
-        <v>114</v>
-      </c>
-      <c r="G70" s="23" t="s">
-        <v>125</v>
+        <v>28.307759372275502</v>
+      </c>
+      <c r="B70">
+        <v>32469.059000000001</v>
+      </c>
+      <c r="C70">
+        <v>3.2469000000000001</v>
+      </c>
+      <c r="D70" s="13">
+        <v>0.1147</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G70" s="24" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
         <f>C71/D71</f>
-        <v>97.714285714285722</v>
+        <v>28.310798946444251</v>
       </c>
       <c r="B71">
-        <v>38303.574000000001</v>
-      </c>
-      <c r="C71">
-        <v>3.8304</v>
+        <v>32246.17</v>
+      </c>
+      <c r="C71" s="11">
+        <v>3.2246000000000001</v>
       </c>
       <c r="D71" s="13">
-        <v>3.9199999999999999E-2</v>
+        <v>0.1139</v>
       </c>
       <c r="E71" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G71" s="24" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
         <f>C72/D72</f>
-        <v>107.72607260726072</v>
+        <v>29.261187214611876</v>
       </c>
       <c r="B72">
-        <v>32641.157999999999</v>
-      </c>
-      <c r="C72" s="11">
-        <v>3.2641</v>
+        <v>32040.548999999999</v>
+      </c>
+      <c r="C72">
+        <v>3.2040999999999999</v>
       </c>
       <c r="D72" s="13">
-        <v>3.0300000000000001E-2</v>
+        <v>0.10949999999999999</v>
       </c>
       <c r="E72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
         <f>C73/D73</f>
-        <v>112.80858085808582</v>
+        <v>97.714285714285722</v>
       </c>
       <c r="B73">
-        <v>34181.218999999997</v>
+        <v>38303.574000000001</v>
       </c>
       <c r="C73">
-        <v>3.4180999999999999</v>
+        <v>3.8304</v>
       </c>
       <c r="D73" s="13">
-        <v>3.0299999999999997E-2</v>
+        <v>3.9199999999999999E-2</v>
       </c>
       <c r="E73" t="s">
         <v>9</v>
@@ -8460,22 +8495,22 @@
         <v>0</v>
       </c>
       <c r="G73" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
         <f>C74/D74</f>
-        <v>112.94267515923566</v>
+        <v>112.80858085808582</v>
       </c>
       <c r="B74">
-        <v>35463.711000000003</v>
+        <v>34181.218999999997</v>
       </c>
       <c r="C74">
-        <v>3.5464000000000002</v>
+        <v>3.4180999999999999</v>
       </c>
       <c r="D74" s="13">
-        <v>3.1400000000000004E-2</v>
+        <v>3.0299999999999997E-2</v>
       </c>
       <c r="E74" t="s">
         <v>9</v>
@@ -8484,22 +8519,22 @@
         <v>0</v>
       </c>
       <c r="G74" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75">
         <f>C75/D75</f>
-        <v>138.48124999999999</v>
+        <v>112.94267515923566</v>
       </c>
       <c r="B75">
-        <v>66471.383000000002</v>
-      </c>
-      <c r="C75" s="11">
-        <v>6.6471</v>
+        <v>35463.711000000003</v>
+      </c>
+      <c r="C75">
+        <v>3.5464000000000002</v>
       </c>
       <c r="D75" s="13">
-        <v>4.8000000000000001E-2</v>
+        <v>3.1400000000000004E-2</v>
       </c>
       <c r="E75" t="s">
         <v>9</v>
@@ -8508,31 +8543,31 @@
         <v>0</v>
       </c>
       <c r="G75" s="24" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
         <f>C76/D76</f>
-        <v>148.68493150684932</v>
+        <v>138.48124999999999</v>
       </c>
       <c r="B76">
-        <v>32561.620999999999</v>
+        <v>66471.383000000002</v>
       </c>
       <c r="C76" s="11">
-        <v>3.2562000000000002</v>
+        <v>6.6471</v>
       </c>
       <c r="D76" s="13">
-        <v>2.1899999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E76" t="s">
         <v>9</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G76" s="24" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -8541,7 +8576,7 @@
   </sheetData>
   <autoFilter ref="A2:G67" xr:uid="{A1C92FFF-D1FD-47B8-800D-712537A126E1}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G76">
-      <sortCondition ref="A2:A67"/>
+      <sortCondition descending="1" ref="F2:F67"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>